<commit_message>
Excel Update untuk Cust Married
</commit_message>
<xml_diff>
--- a/Excel/3. CustomerDataCompletion-Personal - Customer.xlsx
+++ b/Excel/3. CustomerDataCompletion-Personal - Customer.xlsx
@@ -1,46 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fendy.tio\git\NAP-CF4WFINAL\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\git\NAP-CF4W-UF\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="644" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="644" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="1.CustomerDetail" r:id="rId1" sheetId="1"/>
-    <sheet name="2.AddressInformation" r:id="rId2" sheetId="2"/>
-    <sheet name="3.JobData" r:id="rId3" sheetId="3"/>
-    <sheet name="4.EmergencyContact" r:id="rId4" sheetId="4"/>
-    <sheet name="5.FinancialData" r:id="rId5" sheetId="5"/>
-    <sheet name="6.CustomerAsset" r:id="rId6" sheetId="6"/>
-    <sheet name="7.OtherAttribute" r:id="rId7" sheetId="7"/>
-    <sheet name="Master" r:id="rId8" sheetId="8"/>
+    <sheet name="1.CustomerDetail" sheetId="1" r:id="rId1"/>
+    <sheet name="2.AddressInformation" sheetId="2" r:id="rId2"/>
+    <sheet name="3.JobData" sheetId="3" r:id="rId3"/>
+    <sheet name="4.EmergencyContact" sheetId="4" r:id="rId4"/>
+    <sheet name="5.FinancialData" sheetId="5" r:id="rId5"/>
+    <sheet name="6.CustomerAsset" sheetId="6" r:id="rId6"/>
+    <sheet name="7.OtherAttribute" sheetId="7" r:id="rId7"/>
+    <sheet name="Master" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_1">Master!$A$1:$B$95</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_10">Master!$AB$1:$AC$16</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_11">Master!$AE$1:$AF$492</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_12">Master!$AH$1:$AI$10</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_13">Master!$AK$1:$AL$3</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_14">Master!$AN$1:$AO$9</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_15">Master!$AQ$1:$AR$2</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_16">Master!$AT$1:$AU$8</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_17">Master!$AW$1:$AX$263</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_18">Master!$BA$1:$BB$242</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_19">Master!$BE$1:$BE$10</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_2">Master!$E$1:$E$30</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_3">Master!$H$1:$H$14</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_4">Master!$J$1:$K$147</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_5">Master!$M$1:$N$315</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_6">Master!$P$1:$Q$6</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_7">Master!$S$1:$T$175</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_8">Master!$V$1:$W$14</definedName>
-    <definedName hidden="1" localSheetId="7" name="ExternalData_9">Master!$Y$1:$Z$193</definedName>
+    <definedName name="ExternalData_1" localSheetId="7" hidden="1">Master!$A$1:$B$95</definedName>
+    <definedName name="ExternalData_10" localSheetId="7" hidden="1">Master!$AB$1:$AC$16</definedName>
+    <definedName name="ExternalData_11" localSheetId="7" hidden="1">Master!$AE$1:$AF$492</definedName>
+    <definedName name="ExternalData_12" localSheetId="7" hidden="1">Master!$AH$1:$AI$10</definedName>
+    <definedName name="ExternalData_13" localSheetId="7" hidden="1">Master!$AK$1:$AL$3</definedName>
+    <definedName name="ExternalData_14" localSheetId="7" hidden="1">Master!$AN$1:$AO$9</definedName>
+    <definedName name="ExternalData_15" localSheetId="7" hidden="1">Master!$AQ$1:$AR$2</definedName>
+    <definedName name="ExternalData_16" localSheetId="7" hidden="1">Master!$AT$1:$AU$8</definedName>
+    <definedName name="ExternalData_17" localSheetId="7" hidden="1">Master!$AW$1:$AX$263</definedName>
+    <definedName name="ExternalData_18" localSheetId="7" hidden="1">Master!$BA$1:$BB$242</definedName>
+    <definedName name="ExternalData_19" localSheetId="7" hidden="1">Master!$BE$1:$BE$10</definedName>
+    <definedName name="ExternalData_2" localSheetId="7" hidden="1">Master!$E$1:$E$30</definedName>
+    <definedName name="ExternalData_3" localSheetId="7" hidden="1">Master!$H$1:$H$14</definedName>
+    <definedName name="ExternalData_4" localSheetId="7" hidden="1">Master!$J$1:$K$147</definedName>
+    <definedName name="ExternalData_5" localSheetId="7" hidden="1">Master!$M$1:$N$315</definedName>
+    <definedName name="ExternalData_6" localSheetId="7" hidden="1">Master!$P$1:$Q$6</definedName>
+    <definedName name="ExternalData_7" localSheetId="7" hidden="1">Master!$S$1:$T$175</definedName>
+    <definedName name="ExternalData_8" localSheetId="7" hidden="1">Master!$V$1:$W$14</definedName>
+    <definedName name="ExternalData_9" localSheetId="7" hidden="1">Master!$Y$1:$Z$193</definedName>
     <definedName name="ListAfWiMult">Master!$AB$2:INDEX(Master!$AB:$AB,SUMPRODUCT(--(Master!$AB:$AB&lt;&gt;"")))</definedName>
     <definedName name="ListAuthorityAML">Master!$AN$2:INDEX(Master!$AN:$AN,SUMPRODUCT(--(Master!$AN:$AN&lt;&gt;"")))</definedName>
     <definedName name="ListBank">Master!$J$2:INDEX(Master!$J:$J,SUMPRODUCT(--(Master!$J:$J&lt;&gt;"")))</definedName>
@@ -62,7 +62,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -75,7 +75,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A16" shapeId="0">
+    <comment ref="A16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A19" shapeId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +167,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A13" shapeId="0">
+    <comment ref="A13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A66" shapeId="0">
+    <comment ref="A66" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A93" shapeId="0">
+    <comment ref="A93" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A8" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -283,7 +283,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A28" shapeId="0">
+    <comment ref="A28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A31" shapeId="0">
+    <comment ref="A31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -398,7 +398,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4543" uniqueCount="4178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4540" uniqueCount="4179">
   <si>
     <t>Full Name</t>
   </si>
@@ -12932,6 +12932,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Spouse Monthly Income</t>
   </si>
 </sst>
 </file>
@@ -13083,92 +13086,92 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="3" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="3" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="3" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="3" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="70">
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -13187,7 +13190,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13196,7 +13199,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13221,7 +13224,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13230,7 +13233,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13261,17 +13264,17 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13296,24 +13299,24 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13322,7 +13325,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13331,10 +13334,10 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13343,7 +13346,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13368,7 +13371,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13377,7 +13380,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13402,7 +13405,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13411,7 +13414,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13436,24 +13439,24 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13462,7 +13465,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13471,27 +13474,27 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13500,7 +13503,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13509,27 +13512,27 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13538,20 +13541,20 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13560,7 +13563,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13577,7 +13580,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13586,7 +13589,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13595,7 +13598,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13612,7 +13615,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13621,7 +13624,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13630,7 +13633,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13647,7 +13650,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13656,7 +13659,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13665,7 +13668,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13690,7 +13693,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13707,7 +13710,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13724,24 +13727,24 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt formatCode="General" numFmtId="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13750,7 +13753,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13759,7 +13762,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13783,7 +13786,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -14002,208 +14005,208 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="65" displayName="Query_Job_Profession" headerRowDxfId="66" id="1" insertRowShift="1" name="Query_Job_Profession" ref="A1:B95" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Query_Job_Profession" displayName="Query_Job_Profession" ref="A1:B95" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A1:B95"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="64" id="1" name="JOB PROFESSION NAME" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="63" id="2" name="JOB POSITION CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="JOB PROFESSION NAME" queryTableFieldId="1" dataDxfId="64"/>
+    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="63"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="33" displayName="Query_Affiliate_with_Multifinance" headerRowDxfId="34" id="10" insertRowShift="1" name="Query_Affiliate_with_Multifinance" ref="AB1:AC16" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Query_Affiliate_with_Multifinance" displayName="Query_Affiliate_with_Multifinance" ref="AB1:AC16" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="AB1:AC16"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="32" id="1" name="AFFILIATE WITH MULTIFINANCE SLIK" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="31" id="2" name="CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="AFFILIATE WITH MULTIFINANCE SLIK" queryTableFieldId="1" dataDxfId="32"/>
+    <tableColumn id="2" uniqueName="2" name="CODE" queryTableFieldId="2" dataDxfId="31"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="29" displayName="Query_Department_AML" headerRowDxfId="30" id="11" insertRowShift="1" name="Query_Department_AML" ref="AE1:AF492" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Query_Department_AML" displayName="Query_Department_AML" ref="AE1:AF492" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="AE1:AF492"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="28" id="1" name="DEPARTMENT AML" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="27" id="2" name="DEPARTMENT AML CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="DEPARTMENT AML" queryTableFieldId="1" dataDxfId="28"/>
+    <tableColumn id="2" uniqueName="2" name="DEPARTMENT AML CODE" queryTableFieldId="2" dataDxfId="27"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="25" displayName="Query_csp_usl_source_aml" headerRowDxfId="26" id="12" insertRowShift="1" name="Query_csp_usl_source_aml" ref="AH1:AI10" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Query_csp_usl_source_aml" displayName="Query_csp_usl_source_aml" ref="AH1:AI10" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="AH1:AI10"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="24" id="1" name="CSP/USL SOURCE AML" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="23" id="2" name="CSP/USL SOURCE AML CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="CSP/USL SOURCE AML" queryTableFieldId="1" dataDxfId="24"/>
+    <tableColumn id="2" uniqueName="2" name="CSP/USL SOURCE AML CODE" queryTableFieldId="2" dataDxfId="23"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="21" displayName="Query_payment_type_aml" headerRowDxfId="22" id="13" insertRowShift="1" name="Query_payment_type_aml" ref="AK1:AL3" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Query_payment_type_aml" displayName="Query_payment_type_aml" ref="AK1:AL3" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="AK1:AL3"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="20" id="1" name="PAYMENT TYPE AML" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="19" id="2" name="CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="PAYMENT TYPE AML" queryTableFieldId="1" dataDxfId="20"/>
+    <tableColumn id="2" uniqueName="2" name="CODE" queryTableFieldId="2" dataDxfId="19"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="17" displayName="Query_authority_aml" headerRowDxfId="18" id="14" insertRowShift="1" name="Query_authority_aml" ref="AN1:AO9" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Query_authority_aml" displayName="Query_authority_aml" ref="AN1:AO9" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="AN1:AO9"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="16" id="1" name="AUTHORITY AML" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="15" id="2" name="AUTHORITY AML2" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="AUTHORITY AML" queryTableFieldId="1" dataDxfId="16"/>
+    <tableColumn id="2" uniqueName="2" name="AUTHORITY AML2" queryTableFieldId="2" dataDxfId="15"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="13" displayName="Query_Business_Source" headerRowDxfId="14" id="15" insertRowShift="1" name="Query_Business_Source" ref="AQ1:AR2" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Query_Business_Source" displayName="Query_Business_Source" ref="AQ1:AR2" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="AQ1:AR2"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="12" id="1" name="BUSINESS SOURCE AML" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="11" id="2" name="CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="BUSINESS SOURCE AML" queryTableFieldId="1" dataDxfId="12"/>
+    <tableColumn id="2" uniqueName="2" name="CODE" queryTableFieldId="2" dataDxfId="11"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="9" displayName="query_building" headerRowDxfId="10" id="16" insertRowShift="1" name="query_building" ref="AT1:AU8" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="query_building" displayName="query_building" ref="AT1:AU8" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="AT1:AU8"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="8" id="1" name="BUILDING" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="7" id="2" name="BUILDING CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="BUILDING" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" uniqueName="2" name="BUILDING CODE" queryTableFieldId="2" dataDxfId="7"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="5" displayName="Query_Industry_Type" headerRowDxfId="6" id="17" insertRowShift="1" name="Query_Industry_Type" ref="AW1:AX263" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Query_Industry_Type" displayName="Query_Industry_Type" ref="AW1:AX263" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="AW1:AX263"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="4" id="1" name="INDUSTRY TYPE NAME" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="3" id="2" name="INDUSTRY TYPE CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="INDUSTRY TYPE NAME" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="2" uniqueName="2" name="INDUSTRY TYPE CODE" queryTableFieldId="2" dataDxfId="3"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Query_Country" headerRowDxfId="2" id="18" name="Query_Country" ref="BA1:BB242" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Query_Country" displayName="Query_Country" ref="BA1:BB242" tableType="queryTable" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="BA1:BB242"/>
   <tableColumns count="2">
-    <tableColumn id="5" name="COUNTRY NAME" queryTableFieldId="1" uniqueName="5"/>
-    <tableColumn id="6" name="COUNTRY CODE" queryTableFieldId="2" uniqueName="6"/>
+    <tableColumn id="5" uniqueName="5" name="COUNTRY NAME" queryTableFieldId="1"/>
+    <tableColumn id="6" uniqueName="6" name="COUNTRY CODE" queryTableFieldId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Query_Copy_Address_From" headerRowDxfId="1" id="19" name="Query_Copy_Address_From" ref="BE1:BE10" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Query_Copy_Address_From" displayName="Query_Copy_Address_From" ref="BE1:BE10" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="BE1:BE10"/>
   <tableColumns count="1">
-    <tableColumn dataDxfId="0" id="3" name="Copy Address" queryTableFieldId="1" uniqueName="3"/>
+    <tableColumn id="3" uniqueName="3" name="Copy Address" queryTableFieldId="1" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Query_Job_Position" headerRowDxfId="62" id="2" name="Query_Job_Position" ref="E1:E30" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Query_Job_Position" displayName="Query_Job_Position" ref="E1:E30" tableType="queryTable" totalsRowShown="0" headerRowDxfId="62">
   <autoFilter ref="E1:E30"/>
   <tableColumns count="1">
-    <tableColumn dataDxfId="61" id="1" name="JOB POSITION NAME" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn id="1" uniqueName="1" name="JOB POSITION NAME" queryTableFieldId="1" dataDxfId="61"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Query_Customer_Relationship" headerRowDxfId="60" id="3" name="Query_Customer_Relationship" ref="H1:H14" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Query_Customer_Relationship" displayName="Query_Customer_Relationship" ref="H1:H14" tableType="queryTable" totalsRowShown="0" headerRowDxfId="60">
   <autoFilter ref="H1:H14"/>
   <tableColumns count="1">
-    <tableColumn dataDxfId="59" id="1" name="Customer Relationship" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn id="1" uniqueName="1" name="Customer Relationship" queryTableFieldId="1" dataDxfId="59"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="57" displayName="Query_Bank" headerRowDxfId="58" id="4" insertRowShift="1" name="Query_Bank" ref="J1:K147" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Query_Bank" displayName="Query_Bank" ref="J1:K147" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="J1:K147"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="56" id="1" name="BANK NAME" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="55" id="2" name="BANK CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="BANK NAME" queryTableFieldId="1" dataDxfId="56"/>
+    <tableColumn id="2" uniqueName="2" name="BANK CODE" queryTableFieldId="2" dataDxfId="55"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="53" displayName="Query_Debtor_Group" headerRowDxfId="54" id="5" insertRowShift="1" name="Query_Debtor_Group" ref="M1:N315" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Query_Debtor_Group" displayName="Query_Debtor_Group" ref="M1:N315" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="M1:N315"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="52" id="1" name="DEBTOR GROUP NAME" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="51" id="2" name="DEBTOR GROUP CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="DEBTOR GROUP NAME" queryTableFieldId="1" dataDxfId="52"/>
+    <tableColumn id="2" uniqueName="2" name="DEBTOR GROUP CODE" queryTableFieldId="2" dataDxfId="51"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="49" displayName="Query_Debtor_Business_Scale" headerRowDxfId="50" id="6" insertRowShift="1" name="Query_Debtor_Business_Scale" ref="P1:Q6" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Query_Debtor_Business_Scale" displayName="Query_Debtor_Business_Scale" ref="P1:Q6" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="P1:Q6"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="48" id="1" name="Debtor Business Scale Description" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="47" id="2" name="Debtor Group Code" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="Debtor Business Scale Description" queryTableFieldId="1" dataDxfId="48"/>
+    <tableColumn id="2" uniqueName="2" name="Debtor Group Code" queryTableFieldId="2" dataDxfId="47"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="45" displayName="Query_Counterpart" headerRowDxfId="46" id="7" insertRowShift="1" name="Query_Counterpart" ref="S1:T175" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Query_Counterpart" displayName="Query_Counterpart" ref="S1:T175" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="S1:T175"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="44" id="1" name="Counterpart Category" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="43" id="2" name="LBPP CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="Counterpart Category" queryTableFieldId="1" dataDxfId="44"/>
+    <tableColumn id="2" uniqueName="2" name="LBPP CODE" queryTableFieldId="2" dataDxfId="43"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="41" displayName="Query_Sustainable_Financial" headerRowDxfId="42" id="8" insertRowShift="1" name="Query_Sustainable_Financial" ref="V1:W14" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Query_Sustainable_Financial" displayName="Query_Sustainable_Financial" ref="V1:W14" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="V1:W14"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="40" id="1" name="Sustainable Financial Business" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="39" id="2" name="LBPP Code" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="Sustainable Financial Business" queryTableFieldId="1" dataDxfId="40"/>
+    <tableColumn id="2" uniqueName="2" name="LBPP Code" queryTableFieldId="2" dataDxfId="39"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="37" displayName="Query_debtor_group_slik" headerRowDxfId="38" id="9" insertRowShift="1" name="Query_debtor_group_slik" ref="Y1:Z193" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Query_debtor_group_slik" displayName="Query_debtor_group_slik" ref="Y1:Z193" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="Y1:Z193"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="36" id="1" name="DEBTOR GROUP SLIK" queryTableFieldId="1" uniqueName="1"/>
-    <tableColumn dataDxfId="35" id="2" name="DEBTOR GROUP SLIK CODE" queryTableFieldId="2" uniqueName="2"/>
+    <tableColumn id="1" uniqueName="1" name="DEBTOR GROUP SLIK" queryTableFieldId="1" dataDxfId="36"/>
+    <tableColumn id="2" uniqueName="2" name="DEBTOR GROUP SLIK CODE" queryTableFieldId="2" dataDxfId="35"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -14212,10 +14215,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -14250,7 +14253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -14285,7 +14288,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -14379,21 +14382,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -14410,7 +14413,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -14462,15 +14465,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -14478,13 +14481,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -14501,7 +14504,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -14518,7 +14521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -14529,7 +14532,7 @@
         <v>4176</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -14544,7 +14547,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -14559,7 +14562,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row customFormat="1" r="6" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -14574,7 +14577,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -14591,7 +14594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" r="8" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -14608,7 +14611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" r="9" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -14625,7 +14628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" r="10" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -14633,7 +14636,7 @@
         <v>4167</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>14</v>
       </c>
@@ -14650,17 +14653,17 @@
         <v>15</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row customFormat="1" r="14" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>18</v>
       </c>
@@ -14677,7 +14680,7 @@
         <v>19</v>
       </c>
     </row>
-    <row customFormat="1" r="15" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>3645</v>
       </c>
@@ -14698,7 +14701,7 @@
         <v>COUNTRY001</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>20</v>
       </c>
@@ -14721,7 +14724,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>21</v>
       </c>
@@ -14738,7 +14741,7 @@
         <v>4143</v>
       </c>
     </row>
-    <row customFormat="1" r="18" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>22</v>
       </c>
@@ -14755,7 +14758,7 @@
         <v>4145</v>
       </c>
     </row>
-    <row customFormat="1" r="19" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
         <v>23</v>
       </c>
@@ -14780,65 +14783,65 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15:XFD16">
-    <cfRule dxfId="69" priority="2" type="expression">
+    <cfRule type="expression" dxfId="69" priority="2">
       <formula>AND(A$14&lt;&gt;"Foreigner",A$14&lt;&gt;"",A$14&lt;&gt;"Nationality")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:XFD19">
-    <cfRule dxfId="68" priority="1" type="expression">
+    <cfRule type="expression" dxfId="68" priority="1">
       <formula>A$8="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F18:K18" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:K18">
       <formula1>"Buddha, Catholic, Christian, Hindu, Islam, Kong Hu Cu"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F17:K17" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:K17">
       <formula1>"S1, S2, S3, SD, SMP, SMA"</formula1>
     </dataValidation>
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="B10:K10"/>
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="B7:K9" type="list">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B10:K10"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B7:K9">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="F14:K14" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F14:K14">
       <formula1>"Local, Foreigner"</formula1>
     </dataValidation>
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="F11:K11" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F11:K11">
       <formula1>"Mr, Mrs, Ms"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B14:E14" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:E14">
       <formula1>"Local, Foreigner"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B11:E11" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:E11">
       <formula1>"Mr, Mrs, Ms"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B15:E15" type="custom">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:E15">
       <formula1>B$14="Foreigner"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B19:E19" type="custom">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19:E19">
       <formula1>B$8="Yes"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4:B5" type="whole">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B5">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
       <formula1>IF(B$14="Foreigner",ListCountry)</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B17:E17" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:E17">
       <formula1>"S1, S2, S3, SD, SMP, SMA, D3"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B18:E18" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:E18">
       <formula1>"Buddha, Catholic, Christian, Hindu, Islam, Kong Hu Cu, AGNOSTIK"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>IF(C$14="Foreigner",Master!$BA$2:$BA$342)</xm:f>
           </x14:formula1>
@@ -14851,20 +14854,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="2" max="5" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -14881,7 +14884,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>25</v>
       </c>
@@ -14898,7 +14901,7 @@
         <v>26</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -14917,7 +14920,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>28</v>
       </c>
@@ -14940,7 +14943,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>32</v>
       </c>
@@ -14963,7 +14966,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row customFormat="1" r="6" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>33</v>
       </c>
@@ -14986,7 +14989,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>34</v>
       </c>
@@ -15009,7 +15012,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row customFormat="1" r="8" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>37</v>
       </c>
@@ -15032,7 +15035,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row customFormat="1" r="9" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>35</v>
       </c>
@@ -15055,7 +15058,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row customFormat="1" r="10" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>38</v>
       </c>
@@ -15078,7 +15081,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>291</v>
       </c>
@@ -15093,7 +15096,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>292</v>
       </c>
@@ -15108,7 +15111,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row customFormat="1" r="13" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>293</v>
       </c>
@@ -15123,7 +15126,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row customFormat="1" r="14" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>294</v>
       </c>
@@ -15138,7 +15141,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row customFormat="1" r="15" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>295</v>
       </c>
@@ -15153,7 +15156,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>296</v>
       </c>
@@ -15168,7 +15171,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>297</v>
       </c>
@@ -15183,7 +15186,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row customFormat="1" r="18" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>298</v>
       </c>
@@ -15198,7 +15201,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row customFormat="1" r="19" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>299</v>
       </c>
@@ -15213,7 +15216,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row customFormat="1" r="20" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>300</v>
       </c>
@@ -15228,7 +15231,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row customFormat="1" r="21" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>301</v>
       </c>
@@ -15243,7 +15246,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row customFormat="1" r="22" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>40</v>
       </c>
@@ -15262,36 +15265,36 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:XFD10">
-    <cfRule dxfId="67" priority="1" type="expression">
+    <cfRule type="expression" dxfId="67" priority="1">
       <formula>AND(A$3&lt;&gt;"",A$3&lt;&gt;"Copy Address From")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="B22:K22" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B22:K22">
       <formula1>"Dinas, Family, KPR, Rented, Self - Owned"</formula1>
     </dataValidation>
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="B2:K2" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:K2">
       <formula1>"Legal, Mailing, Residence, Residence 2"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="I3:K3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:K3">
       <formula1>"Job, Legal, Residence"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4:B10" type="custom">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B10">
       <formula1>ISBLANK(B$3)</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$BE$2:$BE$110</xm:f>
           </x14:formula1>
           <xm:sqref>C3:H3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$BE$2:$BE$20</xm:f>
           </x14:formula1>
@@ -15304,20 +15307,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:L114"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K114"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
-    <col min="2" max="5" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="24" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -15334,7 +15337,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>3633</v>
       </c>
@@ -15349,7 +15352,7 @@
       <c r="J2" s="44"/>
       <c r="K2" s="45"/>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>42</v>
       </c>
@@ -15376,7 +15379,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>99</v>
       </c>
@@ -15399,7 +15402,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>44</v>
       </c>
@@ -15422,7 +15425,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row customFormat="1" r="6" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>47</v>
       </c>
@@ -15445,7 +15448,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
@@ -15462,7 +15465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" r="8" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -15479,7 +15482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" r="9" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>280</v>
       </c>
@@ -15487,7 +15490,7 @@
         <v>51</v>
       </c>
     </row>
-    <row customFormat="1" r="10" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>281</v>
       </c>
@@ -15505,7 +15508,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>282</v>
       </c>
@@ -15522,7 +15525,7 @@
         <v>3092</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -15536,7 +15539,7 @@
         <v>53</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>54</v>
       </c>
@@ -15559,7 +15562,7 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
     </row>
-    <row customFormat="1" r="14" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>283</v>
       </c>
@@ -15580,7 +15583,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row customFormat="1" r="15" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -15601,12 +15604,12 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row customFormat="1" r="16" s="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
         <v>4146</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>42</v>
       </c>
@@ -15627,7 +15630,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row customFormat="1" r="18" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>99</v>
       </c>
@@ -15638,7 +15641,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row customFormat="1" r="19" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -15646,12 +15649,12 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" r="20" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row customFormat="1" r="21" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>4147</v>
       </c>
@@ -15672,7 +15675,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row customFormat="1" r="22" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>4148</v>
       </c>
@@ -15680,7 +15683,7 @@
         <v>4149</v>
       </c>
     </row>
-    <row customFormat="1" r="23" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>4150</v>
       </c>
@@ -15688,7 +15691,7 @@
         <v>1823612693</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>4151</v>
       </c>
@@ -15696,7 +15699,7 @@
         <v>44056</v>
       </c>
     </row>
-    <row customFormat="1" r="25" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>283</v>
       </c>
@@ -15704,12 +15707,12 @@
         <v>311</v>
       </c>
     </row>
-    <row customFormat="1" r="26" s="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>4152</v>
       </c>
     </row>
-    <row customFormat="1" r="27" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
         <v>42</v>
       </c>
@@ -15718,7 +15721,7 @@
         <v>CLG_STD</v>
       </c>
     </row>
-    <row customFormat="1" r="28" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>99</v>
       </c>
@@ -15726,17 +15729,17 @@
         <v>175</v>
       </c>
     </row>
-    <row customFormat="1" r="29" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row customFormat="1" r="30" s="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
         <v>4153</v>
       </c>
     </row>
-    <row customFormat="1" r="31" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>42</v>
       </c>
@@ -15745,7 +15748,7 @@
         <v>ENTR</v>
       </c>
     </row>
-    <row customFormat="1" r="32" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>99</v>
       </c>
@@ -15753,7 +15756,7 @@
         <v>276</v>
       </c>
     </row>
-    <row customFormat="1" r="33" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>44</v>
       </c>
@@ -15761,7 +15764,7 @@
         <v>302</v>
       </c>
     </row>
-    <row customFormat="1" r="34" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>50</v>
       </c>
@@ -15769,7 +15772,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" r="35" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>280</v>
       </c>
@@ -15777,7 +15780,7 @@
         <v>4154</v>
       </c>
     </row>
-    <row customFormat="1" r="36" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>4147</v>
       </c>
@@ -15786,7 +15789,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row customFormat="1" r="37" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>4148</v>
       </c>
@@ -15794,12 +15797,12 @@
         <v>4155</v>
       </c>
     </row>
-    <row customFormat="1" r="38" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>4156</v>
       </c>
     </row>
-    <row customFormat="1" r="39" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>4157</v>
       </c>
@@ -15807,7 +15810,7 @@
         <v>4158</v>
       </c>
     </row>
-    <row customFormat="1" r="40" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>283</v>
       </c>
@@ -15815,7 +15818,7 @@
         <v>3373</v>
       </c>
     </row>
-    <row customFormat="1" r="41" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -15823,12 +15826,12 @@
         <v>500</v>
       </c>
     </row>
-    <row customFormat="1" r="42" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>4159</v>
       </c>
     </row>
-    <row customFormat="1" r="43" s="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="43" t="s">
         <v>3634</v>
       </c>
@@ -15843,7 +15846,7 @@
       <c r="J43" s="44"/>
       <c r="K43" s="45"/>
     </row>
-    <row customFormat="1" r="44" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>28</v>
       </c>
@@ -15860,7 +15863,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" r="45" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>32</v>
       </c>
@@ -15883,7 +15886,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row customFormat="1" r="46" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
         <v>33</v>
       </c>
@@ -15906,7 +15909,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row customFormat="1" r="47" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
         <v>34</v>
       </c>
@@ -15929,7 +15932,7 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row customFormat="1" r="48" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
         <v>35</v>
       </c>
@@ -15952,7 +15955,7 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row customFormat="1" r="49" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
         <v>37</v>
       </c>
@@ -15975,7 +15978,7 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row customFormat="1" r="50" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>38</v>
       </c>
@@ -15998,7 +16001,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row customFormat="1" r="51" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>39</v>
       </c>
@@ -16013,7 +16016,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row customFormat="1" r="52" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>291</v>
       </c>
@@ -16028,7 +16031,7 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row customFormat="1" r="53" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>292</v>
       </c>
@@ -16043,7 +16046,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row customFormat="1" r="54" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>293</v>
       </c>
@@ -16058,7 +16061,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row customFormat="1" r="55" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>294</v>
       </c>
@@ -16073,7 +16076,7 @@
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row customFormat="1" r="56" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>295</v>
       </c>
@@ -16088,7 +16091,7 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row customFormat="1" r="57" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>296</v>
       </c>
@@ -16103,7 +16106,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row customFormat="1" r="58" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>297</v>
       </c>
@@ -16118,7 +16121,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row customFormat="1" r="59" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>298</v>
       </c>
@@ -16133,7 +16136,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
-    <row customFormat="1" r="60" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>299</v>
       </c>
@@ -16148,7 +16151,7 @@
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row customFormat="1" r="61" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>300</v>
       </c>
@@ -16163,7 +16166,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row customFormat="1" r="62" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>301</v>
       </c>
@@ -16178,7 +16181,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row customFormat="1" r="63" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>40</v>
       </c>
@@ -16192,7 +16195,7 @@
         <v>41</v>
       </c>
     </row>
-    <row customFormat="1" r="64" s="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
         <v>3635</v>
       </c>
@@ -16207,18 +16210,18 @@
       <c r="J64" s="44"/>
       <c r="K64" s="45"/>
     </row>
-    <row customFormat="1" r="65" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row customFormat="1" r="66" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>285</v>
       </c>
       <c r="B66" s="37"/>
     </row>
-    <row customFormat="1" r="67" s="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="43" t="s">
         <v>3636</v>
       </c>
@@ -16233,7 +16236,7 @@
       <c r="J67" s="44"/>
       <c r="K67" s="45"/>
     </row>
-    <row customFormat="1" r="68" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>345</v>
       </c>
@@ -16250,7 +16253,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" r="69" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>346</v>
       </c>
@@ -16273,7 +16276,7 @@
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row customFormat="1" r="70" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>347</v>
       </c>
@@ -16296,7 +16299,7 @@
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row customFormat="1" r="71" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>348</v>
       </c>
@@ -16319,7 +16322,7 @@
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row customFormat="1" r="72" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>349</v>
       </c>
@@ -16342,7 +16345,7 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row customFormat="1" r="73" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>350</v>
       </c>
@@ -16365,7 +16368,7 @@
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
-    <row customFormat="1" r="74" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>351</v>
       </c>
@@ -16388,7 +16391,7 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row customFormat="1" r="75" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>352</v>
       </c>
@@ -16403,7 +16406,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
-    <row customFormat="1" r="76" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>353</v>
       </c>
@@ -16418,7 +16421,7 @@
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
-    <row customFormat="1" r="77" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>354</v>
       </c>
@@ -16433,7 +16436,7 @@
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row customFormat="1" r="78" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>355</v>
       </c>
@@ -16448,7 +16451,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row customFormat="1" r="79" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>356</v>
       </c>
@@ -16463,7 +16466,7 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row customFormat="1" r="80" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>357</v>
       </c>
@@ -16478,7 +16481,7 @@
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
-    <row customFormat="1" r="81" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>358</v>
       </c>
@@ -16493,7 +16496,7 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
     </row>
-    <row customFormat="1" r="82" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>359</v>
       </c>
@@ -16508,7 +16511,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row customFormat="1" r="83" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>360</v>
       </c>
@@ -16523,7 +16526,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row customFormat="1" r="84" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>361</v>
       </c>
@@ -16538,7 +16541,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row customFormat="1" r="85" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>362</v>
       </c>
@@ -16553,7 +16556,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row customFormat="1" r="86" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>363</v>
       </c>
@@ -16568,7 +16571,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row customFormat="1" r="87" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>364</v>
       </c>
@@ -16582,7 +16585,7 @@
         <v>41</v>
       </c>
     </row>
-    <row customFormat="1" r="88" s="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="43" t="s">
         <v>3637</v>
       </c>
@@ -16597,33 +16600,33 @@
       <c r="J88" s="44"/>
       <c r="K88" s="45"/>
     </row>
-    <row customFormat="1" r="89" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row customFormat="1" r="90" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row customFormat="1" r="91" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row customFormat="1" r="92" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row customFormat="1" r="93" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>289</v>
       </c>
       <c r="B93" s="37"/>
     </row>
-    <row customFormat="1" r="94" s="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="43" t="s">
         <v>3638</v>
       </c>
@@ -16638,7 +16641,7 @@
       <c r="J94" s="44"/>
       <c r="K94" s="45"/>
     </row>
-    <row customFormat="1" r="95" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>325</v>
       </c>
@@ -16652,7 +16655,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" r="96" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>326</v>
       </c>
@@ -16673,7 +16676,7 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
-    <row customFormat="1" r="97" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>327</v>
       </c>
@@ -16694,7 +16697,7 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row customFormat="1" r="98" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>328</v>
       </c>
@@ -16715,7 +16718,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row customFormat="1" r="99" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>329</v>
       </c>
@@ -16729,7 +16732,7 @@
         <v>36</v>
       </c>
     </row>
-    <row customFormat="1" r="100" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>330</v>
       </c>
@@ -16743,7 +16746,7 @@
         <v>36</v>
       </c>
     </row>
-    <row customFormat="1" r="101" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>331</v>
       </c>
@@ -16757,7 +16760,7 @@
         <v>290</v>
       </c>
     </row>
-    <row customFormat="1" r="102" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>332</v>
       </c>
@@ -16772,7 +16775,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
     </row>
-    <row customFormat="1" r="103" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>333</v>
       </c>
@@ -16787,7 +16790,7 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row customFormat="1" r="104" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>334</v>
       </c>
@@ -16802,7 +16805,7 @@
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
     </row>
-    <row customFormat="1" r="105" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>335</v>
       </c>
@@ -16817,7 +16820,7 @@
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
     </row>
-    <row customFormat="1" r="106" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>336</v>
       </c>
@@ -16832,7 +16835,7 @@
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
     </row>
-    <row customFormat="1" r="107" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>337</v>
       </c>
@@ -16847,7 +16850,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
     </row>
-    <row customFormat="1" r="108" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>338</v>
       </c>
@@ -16862,7 +16865,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
     </row>
-    <row customFormat="1" r="109" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>339</v>
       </c>
@@ -16877,7 +16880,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
     </row>
-    <row customFormat="1" r="110" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>340</v>
       </c>
@@ -16892,7 +16895,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
     </row>
-    <row customFormat="1" r="111" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>341</v>
       </c>
@@ -16907,7 +16910,7 @@
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
     </row>
-    <row customFormat="1" r="112" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>342</v>
       </c>
@@ -16922,7 +16925,7 @@
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
     </row>
-    <row customFormat="1" r="113" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>343</v>
       </c>
@@ -16937,7 +16940,7 @@
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
     </row>
-    <row customFormat="1" r="114" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>344</v>
       </c>
@@ -16964,60 +16967,60 @@
     <mergeCell ref="A88:XFD88"/>
   </mergeCells>
   <dataValidations count="9">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:K8 F11:K11 B19:E19 B34" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:K8 F11:K11 B19:E19 B34">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="C87:K87 C63:K63 C114:K114" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C87:K87 C63:K63 C114:K114">
       <formula1>"Dinas, Family, KPR, Rented, Self - Owned"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6:K6" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:K6">
       <formula1>"Contract, Permanent"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B15 B41" type="whole">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B41">
       <formula1>0</formula1>
       <formula2>999999999999999000000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4 B18:E18 B32 B28" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 B18:E18 B32 B28">
       <formula1>ListJobProfession</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B5 B33" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 B33">
       <formula1>ListJobPosition</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B11 B22:E22 B37" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B22:E22 B37">
       <formula1>ListIndustryType</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B63 B87 B114" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63 B87 B114">
       <formula1>"Dinas, Family, KPR, Rented, Self - Owned"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B42" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
       <formula1>"Domestic Investment, Foreign Investment"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>F5:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$A$2:$A$195</xm:f>
           </x14:formula1>
           <xm:sqref>C4:E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$E$2:$E$129</xm:f>
           </x14:formula1>
           <xm:sqref>C5:E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$AW$2:$AW$515</xm:f>
           </x14:formula1>
@@ -17030,8 +17033,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -17039,14 +17042,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -17063,7 +17066,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>365</v>
       </c>
@@ -17071,7 +17074,7 @@
         <v>377</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>58</v>
       </c>
@@ -17094,7 +17097,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>62</v>
       </c>
@@ -17117,7 +17120,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -17130,22 +17133,22 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="F3:K3" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F3:K3">
       <formula1>"AKTA, CAT CAT, CAT IS A CAT, DESCRIPTION FOR AAA, DESCRIPTION FOR ASA, DESCRIPTION FOR KTP, E-KTP, KITAS, NPWP, SIM"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B5:E5" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:E5">
       <formula1>"Job, Legal, Residence"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>ListCusRel</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$H$2:$H$113</xm:f>
           </x14:formula1>
@@ -17158,20 +17161,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="2" max="5" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -17188,7 +17191,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>3639</v>
       </c>
@@ -17203,7 +17206,7 @@
       <c r="J2" s="44"/>
       <c r="K2" s="45"/>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>65</v>
       </c>
@@ -17226,7 +17229,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
@@ -17247,7 +17250,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>67</v>
       </c>
@@ -17270,7 +17273,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row customFormat="1" r="6" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
@@ -17291,7 +17294,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
@@ -17312,7 +17315,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row customFormat="1" r="8" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>379</v>
       </c>
@@ -17335,100 +17338,92 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row customFormat="1" r="9" s="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>4178</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
         <v>3640</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="45"/>
-    </row>
-    <row customFormat="1" r="10" s="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="45"/>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B11" s="39">
         <v>0</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>1000000001</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <v>1000000002</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
         <v>1000000003</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row customFormat="1" r="11" s="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>3641</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row customFormat="1" r="12" s="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="45"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="3">
         <v>192974891</v>
       </c>
-      <c r="C12" s="3" t="str">
-        <f>VLOOKUP(C13,Master!$J$1:$K$204,2,FALSE)</f>
+      <c r="C13" s="3" t="str">
+        <f>VLOOKUP(C14,Master!$J$1:$K$204,2,FALSE)</f>
         <v>014</v>
       </c>
-      <c r="D12" s="3" t="str">
-        <f>VLOOKUP(D13,Master!$J$1:$K$204,2,FALSE)</f>
+      <c r="D13" s="3" t="str">
+        <f>VLOOKUP(D14,Master!$J$1:$K$204,2,FALSE)</f>
         <v>014</v>
       </c>
-      <c r="E12" s="3" t="str">
-        <f>VLOOKUP(E13,Master!$J$1:$K$204,2,FALSE)</f>
+      <c r="E13" s="3" t="str">
+        <f>VLOOKUP(E14,Master!$J$1:$K$204,2,FALSE)</f>
         <v>014</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row customFormat="1" r="13" s="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
-        <v>728</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>390</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -17437,83 +17432,89 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row customFormat="1" r="14" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
+        <v>728</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>4166</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row customFormat="1" r="15" s="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>4165</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>4168</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row customFormat="1" r="17" s="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row customFormat="1" r="18" s="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>11</v>
@@ -17528,61 +17529,78 @@
         <v>11</v>
       </c>
     </row>
-    <row customFormat="1" r="19" s="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
         <v>729</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B20" s="12">
         <v>5000000000</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:XFD2"/>
-    <mergeCell ref="A9:XFD9"/>
-    <mergeCell ref="A11:XFD11"/>
+    <mergeCell ref="A10:XFD10"/>
+    <mergeCell ref="A12:XFD12"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G17:K19 B17:F18" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18:K20 B18:F19">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B5:K5" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:K5">
       <formula1>"Business, Online Shop, Salary, Stock Trading"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B3:B4" type="whole">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+27</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6:B7" type="whole">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+22</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10" type="whole">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B19" type="whole">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+23</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B13" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
       <formula1>ListBank</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$J$2:$J$305</xm:f>
           </x14:formula1>
-          <xm:sqref>C13:E13</xm:sqref>
+          <xm:sqref>C14:E14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -17591,8 +17609,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -17600,11 +17618,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="2" max="5" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -17621,7 +17639,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>85</v>
       </c>
@@ -17635,7 +17653,7 @@
         <v>86</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -17649,7 +17667,7 @@
         <v>88</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>89</v>
       </c>
@@ -17664,7 +17682,7 @@
         <v>600000000</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>90</v>
       </c>
@@ -17681,21 +17699,21 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:E2" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:E2">
       <formula1>"Mobil, Motor, Rumah"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4:E5" type="whole">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:E5">
       <formula1>0</formula1>
       <formula2>999999999999999000000</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
@@ -17703,12 +17721,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="7" width="15.0" collapsed="true"/>
-    <col min="3" max="5" bestFit="true" customWidth="true" style="7" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" style="7" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="14.85546875" style="7" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -17725,7 +17743,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>3642</v>
       </c>
@@ -17734,7 +17752,7 @@
       <c r="D2" s="44"/>
       <c r="E2" s="45"/>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>91</v>
       </c>
@@ -17755,7 +17773,7 @@
         <v>07</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>730</v>
       </c>
@@ -17772,7 +17790,7 @@
         <v>740</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>96</v>
       </c>
@@ -17793,7 +17811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="6" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>731</v>
       </c>
@@ -17810,7 +17828,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>1467</v>
       </c>
@@ -17831,7 +17849,7 @@
         <v>e2955</v>
       </c>
     </row>
-    <row customFormat="1" ht="135" r="8" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>732</v>
       </c>
@@ -17848,7 +17866,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row customFormat="1" r="9" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>1468</v>
       </c>
@@ -17869,7 +17887,7 @@
         <v>e3822</v>
       </c>
     </row>
-    <row customFormat="1" ht="105" r="10" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>733</v>
       </c>
@@ -17886,7 +17904,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
         <v>3643</v>
       </c>
@@ -17895,7 +17913,7 @@
       <c r="D11" s="44"/>
       <c r="E11" s="45"/>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1649</v>
       </c>
@@ -17906,7 +17924,7 @@
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
-    <row customFormat="1" r="13" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>1650</v>
       </c>
@@ -17927,7 +17945,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row customFormat="1" ht="30" r="14" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>1651</v>
       </c>
@@ -17938,7 +17956,7 @@
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
-    <row customFormat="1" r="15" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1652</v>
       </c>
@@ -17949,7 +17967,7 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1653</v>
       </c>
@@ -17960,7 +17978,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
-    <row customFormat="1" r="17" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>1657</v>
       </c>
@@ -17981,7 +17999,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row customFormat="1" ht="45" r="18" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>1654</v>
       </c>
@@ -17992,7 +18010,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row customFormat="1" r="19" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>1656</v>
       </c>
@@ -18013,7 +18031,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row customFormat="1" r="20" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>1655</v>
       </c>
@@ -18024,7 +18042,7 @@
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row customFormat="1" r="21" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
         <v>1659</v>
       </c>
@@ -18045,7 +18063,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row customFormat="1" ht="30" r="22" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>1658</v>
       </c>
@@ -18056,7 +18074,7 @@
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
     </row>
-    <row customFormat="1" ht="45" r="23" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>1660</v>
       </c>
@@ -18077,7 +18095,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row customFormat="1" ht="30" r="24" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>1661</v>
       </c>
@@ -18088,7 +18106,7 @@
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
     </row>
-    <row customFormat="1" r="25" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>1662</v>
       </c>
@@ -18099,7 +18117,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
-    <row customFormat="1" r="26" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>1663</v>
       </c>
@@ -18120,7 +18138,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row customFormat="1" r="27" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1664</v>
       </c>
@@ -18129,7 +18147,7 @@
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
     </row>
-    <row customFormat="1" r="28" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>97</v>
       </c>
@@ -18146,7 +18164,7 @@
         <v>3355</v>
       </c>
     </row>
-    <row customFormat="1" r="29" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>1665</v>
       </c>
@@ -18167,7 +18185,7 @@
         <v>BISNIS_SENDIRI</v>
       </c>
     </row>
-    <row customFormat="1" r="30" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>1666</v>
       </c>
@@ -18184,7 +18202,7 @@
         <v>3055</v>
       </c>
     </row>
-    <row customFormat="1" r="31" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>1667</v>
       </c>
@@ -18201,7 +18219,7 @@
         <v>3354</v>
       </c>
     </row>
-    <row customFormat="1" r="32" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>1668</v>
       </c>
@@ -18221,7 +18239,7 @@
         <v>FAMILY</v>
       </c>
     </row>
-    <row customFormat="1" r="33" s="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>1669</v>
       </c>
@@ -18244,121 +18262,121 @@
     <mergeCell ref="A11:XFD11"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C15:E16 C12:E12 C25:E25" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:E16 C12:E12 C25:E25">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12 B15:B16 B25" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 B15:B16 B25">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>ListDebtGroup</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>ListDebtorBusinessScale</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
       <formula1>ListCounterpart</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
       <formula1>ListSusFinBus</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B14" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
       <formula1>ListDebtGroupSLIK</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B18" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
       <formula1>ListAfWiMult</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B20" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
       <formula1>ListDeptAML</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B22" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
       <formula1>ListCSPUSL</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B24" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
       <formula1>ListPaymentTypeAML</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B27" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
       <formula1>ListAuthorityAML</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B30" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
       <formula1>ListBusinessSource</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B33" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33">
       <formula1>ListBuilding</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$AT$2:$AT$109</xm:f>
           </x14:formula1>
           <xm:sqref>C33:E33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$M$2:$M$629</xm:f>
           </x14:formula1>
           <xm:sqref>C4:E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$P$2:$P$107</xm:f>
           </x14:formula1>
           <xm:sqref>C6:E6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$S$2:$S$349</xm:f>
           </x14:formula1>
           <xm:sqref>C8:E8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$V$2:$V$115</xm:f>
           </x14:formula1>
           <xm:sqref>C10:E10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$Y$2:$Y$385</xm:f>
           </x14:formula1>
           <xm:sqref>C14:E14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$AB$2:$AB$117</xm:f>
           </x14:formula1>
           <xm:sqref>C18:E18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$AE$2:$AE$983</xm:f>
           </x14:formula1>
           <xm:sqref>C20:E20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$AH$2:$AH$111</xm:f>
           </x14:formula1>
           <xm:sqref>C22:E22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$AK$2:$AK$104</xm:f>
           </x14:formula1>
           <xm:sqref>C24:E24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$AN$2:$AN$111</xm:f>
           </x14:formula1>
           <xm:sqref>C27:E27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Master!$AQ$2:$AQ$102</xm:f>
           </x14:formula1>
@@ -18371,8 +18389,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DC882"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DB882"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D92" sqref="D92"/>
@@ -18380,46 +18398,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="15" width="42.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="17" width="30.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="17" width="23.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="17" width="35.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="19" width="18.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="17" width="29.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="17" width="22.85546875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="17" width="33.85546875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="17" width="20.7109375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="17" width="255.7109375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="17" width="12.85546875" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="22" width="80.140625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="17" width="12.5703125" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="23" width="80.7109375" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="20" width="21.5703125" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="23" width="79.85546875" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="20" width="8.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="17" width="89.0" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" style="17" width="25.5703125" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" style="17" width="23.0" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" style="20" width="28.5703125" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="17" width="25.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" style="17" width="31.140625" collapsed="true"/>
-    <col min="40" max="40" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="43" max="43" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="44" max="44" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" style="17" width="12.42578125" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" style="17" width="17.42578125" collapsed="true"/>
-    <col min="48" max="48" style="17" width="9.140625" collapsed="true"/>
-    <col min="49" max="49" customWidth="true" style="17" width="97.7109375" collapsed="true"/>
-    <col min="50" max="50" customWidth="true" style="17" width="22.5703125" collapsed="true"/>
-    <col min="53" max="53" customWidth="true" width="43.28515625" collapsed="true"/>
-    <col min="54" max="54" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="57" max="57" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="1" max="1" width="42.140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" style="14" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30" style="17" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.85546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.85546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.85546875" style="19" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="29.42578125" style="17" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.85546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="33.85546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.7109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="255.7109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.85546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="80.140625" style="22" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.5703125" style="17" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="80.7109375" style="23" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="21.5703125" style="20" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="79.85546875" style="23" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="8.140625" style="20" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="89" style="17" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="25.5703125" style="17" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="23" style="17" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5703125" style="20" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="25.140625" style="17" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="31.140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="12.42578125" style="17" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="17.42578125" style="17" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="9.140625" style="17" collapsed="1"/>
+    <col min="49" max="49" width="97.7109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="22.5703125" style="17" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="43.28515625" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="15.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="30" r="1" s="13" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>3361</v>
       </c>
@@ -19304,7 +19322,7 @@
         <v>4137</v>
       </c>
     </row>
-    <row ht="30" r="10" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>115</v>
       </c>
@@ -19383,7 +19401,7 @@
         <v>4138</v>
       </c>
     </row>
-    <row ht="30" r="11" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:57" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>117</v>
       </c>
@@ -19451,7 +19469,7 @@
         <v>3667</v>
       </c>
     </row>
-    <row ht="30" r="12" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:57" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>119</v>
       </c>
@@ -22815,7 +22833,7 @@
         <v>3797</v>
       </c>
     </row>
-    <row ht="30" r="77" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
         <v>247</v>
       </c>
@@ -22865,7 +22883,7 @@
         <v>3799</v>
       </c>
     </row>
-    <row ht="30" r="78" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
         <v>249</v>
       </c>
@@ -23465,7 +23483,7 @@
         <v>3823</v>
       </c>
     </row>
-    <row ht="30" r="90" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
         <v>271</v>
       </c>
@@ -23515,7 +23533,7 @@
         <v>3825</v>
       </c>
     </row>
-    <row ht="30" r="91" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
         <v>272</v>
       </c>
@@ -24092,7 +24110,7 @@
         <v>3372</v>
       </c>
     </row>
-    <row ht="30" r="103" spans="10:106" x14ac:dyDescent="0.25">
+    <row r="103" spans="10:106" ht="30" x14ac:dyDescent="0.25">
       <c r="J103" s="18" t="s">
         <v>489</v>
       </c>
@@ -24136,7 +24154,7 @@
         <v>3851</v>
       </c>
     </row>
-    <row ht="30" r="104" spans="10:106" x14ac:dyDescent="0.25">
+    <row r="104" spans="10:106" ht="30" x14ac:dyDescent="0.25">
       <c r="J104" s="18" t="s">
         <v>390</v>
       </c>
@@ -24356,7 +24374,7 @@
         <v>3861</v>
       </c>
     </row>
-    <row ht="30" r="109" spans="10:106" x14ac:dyDescent="0.25">
+    <row r="109" spans="10:106" ht="30" x14ac:dyDescent="0.25">
       <c r="J109" s="18" t="s">
         <v>410</v>
       </c>
@@ -24620,7 +24638,7 @@
         <v>3873</v>
       </c>
     </row>
-    <row ht="30" r="115" spans="10:54" x14ac:dyDescent="0.25">
+    <row r="115" spans="10:54" ht="30" x14ac:dyDescent="0.25">
       <c r="J115" s="18" t="s">
         <v>509</v>
       </c>
@@ -24664,7 +24682,7 @@
         <v>3875</v>
       </c>
     </row>
-    <row ht="30" r="116" spans="10:54" x14ac:dyDescent="0.25">
+    <row r="116" spans="10:54" ht="30" x14ac:dyDescent="0.25">
       <c r="J116" s="18" t="s">
         <v>511</v>
       </c>
@@ -25632,7 +25650,7 @@
         <v>3919</v>
       </c>
     </row>
-    <row ht="30" r="138" spans="10:54" x14ac:dyDescent="0.25">
+    <row r="138" spans="10:54" ht="30" x14ac:dyDescent="0.25">
       <c r="J138" s="18" t="s">
         <v>550</v>
       </c>
@@ -26228,7 +26246,7 @@
         <v>3947</v>
       </c>
     </row>
-    <row ht="30" r="152" spans="10:54" x14ac:dyDescent="0.25">
+    <row r="152" spans="10:54" ht="30" x14ac:dyDescent="0.25">
       <c r="K152" s="20"/>
       <c r="M152" s="18" t="s">
         <v>884</v>
@@ -26267,7 +26285,7 @@
         <v>3949</v>
       </c>
     </row>
-    <row ht="30" r="153" spans="10:54" x14ac:dyDescent="0.25">
+    <row r="153" spans="10:54" ht="30" x14ac:dyDescent="0.25">
       <c r="K153" s="20"/>
       <c r="M153" s="18" t="s">
         <v>885</v>
@@ -33123,8 +33141,8 @@
       <c r="AF882" s="20"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="19">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
Revisi error excel AITATR3-72
</commit_message>
<xml_diff>
--- a/Excel/3. CustomerDataCompletion-Personal - Customer.xlsx
+++ b/Excel/3. CustomerDataCompletion-Personal - Customer.xlsx
@@ -1,46 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\git\NAP-CF4W-UF\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="644" firstSheet="2" activeTab="4"/>
+    <workbookView activeTab="4" tabRatio="644" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="1.CustomerDetail" sheetId="1" r:id="rId1"/>
-    <sheet name="2.AddressInformation" sheetId="2" r:id="rId2"/>
-    <sheet name="3.JobData" sheetId="3" r:id="rId3"/>
-    <sheet name="4.EmergencyContact" sheetId="4" r:id="rId4"/>
-    <sheet name="5.FinancialData" sheetId="5" r:id="rId5"/>
-    <sheet name="6.CustomerAsset" sheetId="6" r:id="rId6"/>
-    <sheet name="7.OtherAttribute" sheetId="7" r:id="rId7"/>
-    <sheet name="Master" sheetId="8" r:id="rId8"/>
+    <sheet name="1.CustomerDetail" r:id="rId1" sheetId="1"/>
+    <sheet name="2.AddressInformation" r:id="rId2" sheetId="2"/>
+    <sheet name="3.JobData" r:id="rId3" sheetId="3"/>
+    <sheet name="4.EmergencyContact" r:id="rId4" sheetId="4"/>
+    <sheet name="5.FinancialData" r:id="rId5" sheetId="5"/>
+    <sheet name="6.CustomerAsset" r:id="rId6" sheetId="6"/>
+    <sheet name="7.OtherAttribute" r:id="rId7" sheetId="7"/>
+    <sheet name="Master" r:id="rId8" sheetId="8"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="7" hidden="1">Master!$A$1:$B$95</definedName>
-    <definedName name="ExternalData_10" localSheetId="7" hidden="1">Master!$AB$1:$AC$16</definedName>
-    <definedName name="ExternalData_11" localSheetId="7" hidden="1">Master!$AE$1:$AF$492</definedName>
-    <definedName name="ExternalData_12" localSheetId="7" hidden="1">Master!$AH$1:$AI$10</definedName>
-    <definedName name="ExternalData_13" localSheetId="7" hidden="1">Master!$AK$1:$AL$3</definedName>
-    <definedName name="ExternalData_14" localSheetId="7" hidden="1">Master!$AN$1:$AO$9</definedName>
-    <definedName name="ExternalData_15" localSheetId="7" hidden="1">Master!$AQ$1:$AR$2</definedName>
-    <definedName name="ExternalData_16" localSheetId="7" hidden="1">Master!$AT$1:$AU$8</definedName>
-    <definedName name="ExternalData_17" localSheetId="7" hidden="1">Master!$AW$1:$AX$263</definedName>
-    <definedName name="ExternalData_18" localSheetId="7" hidden="1">Master!$BA$1:$BB$242</definedName>
-    <definedName name="ExternalData_19" localSheetId="7" hidden="1">Master!$BE$1:$BE$10</definedName>
-    <definedName name="ExternalData_2" localSheetId="7" hidden="1">Master!$E$1:$E$30</definedName>
-    <definedName name="ExternalData_3" localSheetId="7" hidden="1">Master!$H$1:$H$14</definedName>
-    <definedName name="ExternalData_4" localSheetId="7" hidden="1">Master!$J$1:$K$147</definedName>
-    <definedName name="ExternalData_5" localSheetId="7" hidden="1">Master!$M$1:$N$315</definedName>
-    <definedName name="ExternalData_6" localSheetId="7" hidden="1">Master!$P$1:$Q$6</definedName>
-    <definedName name="ExternalData_7" localSheetId="7" hidden="1">Master!$S$1:$T$175</definedName>
-    <definedName name="ExternalData_8" localSheetId="7" hidden="1">Master!$V$1:$W$14</definedName>
-    <definedName name="ExternalData_9" localSheetId="7" hidden="1">Master!$Y$1:$Z$193</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_1">Master!$A$1:$B$95</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_10">Master!$AB$1:$AC$16</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_11">Master!$AE$1:$AF$492</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_12">Master!$AH$1:$AI$10</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_13">Master!$AK$1:$AL$3</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_14">Master!$AN$1:$AO$9</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_15">Master!$AQ$1:$AR$2</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_16">Master!$AT$1:$AU$8</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_17">Master!$AW$1:$AX$263</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_18">Master!$BA$1:$BB$242</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_19">Master!$BE$1:$BE$10</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_2">Master!$E$1:$E$30</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_3">Master!$H$1:$H$14</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_4">Master!$J$1:$K$147</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_5">Master!$M$1:$N$315</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_6">Master!$P$1:$Q$6</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_7">Master!$S$1:$T$175</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_8">Master!$V$1:$W$14</definedName>
+    <definedName hidden="1" localSheetId="7" name="ExternalData_9">Master!$Y$1:$Z$193</definedName>
     <definedName name="ListAfWiMult">Master!$AB$2:INDEX(Master!$AB:$AB,SUMPRODUCT(--(Master!$AB:$AB&lt;&gt;"")))</definedName>
     <definedName name="ListAuthorityAML">Master!$AN$2:INDEX(Master!$AN:$AN,SUMPRODUCT(--(Master!$AN:$AN&lt;&gt;"")))</definedName>
     <definedName name="ListBank">Master!$J$2:INDEX(Master!$J:$J,SUMPRODUCT(--(Master!$J:$J&lt;&gt;"")))</definedName>
@@ -62,7 +62,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -75,7 +75,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment ref="A16" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A16" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A19" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +167,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment ref="A13" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A66" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A93" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A93" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -283,7 +283,7 @@
     <author>Jeremy Andreas</author>
   </authors>
   <commentList>
-    <comment ref="A28" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A28" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A31" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -398,7 +398,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4541" uniqueCount="4180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4552" uniqueCount="4178">
   <si>
     <t>Full Name</t>
   </si>
@@ -12817,9 +12817,6 @@
     <t>Previous Job</t>
   </si>
   <si>
-    <t>Ala</t>
-  </si>
-  <si>
     <t>Permanent</t>
   </si>
   <si>
@@ -12922,22 +12919,19 @@
     <t>721382838128</t>
   </si>
   <si>
-    <t>CAL CRUBERG</t>
-  </si>
-  <si>
     <t>WARNING</t>
   </si>
   <si>
     <t>FT RICKY</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Spouse Monthly Income</t>
   </si>
   <si>
     <t>Is Join Income</t>
+  </si>
+  <si>
+    <t>BLI GUNG</t>
   </si>
 </sst>
 </file>
@@ -13089,92 +13083,95 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="49">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="3" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="3" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="3" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="3" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="70">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13193,7 +13190,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13202,7 +13199,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13227,7 +13224,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13236,7 +13233,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13267,17 +13264,17 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13302,24 +13299,24 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13328,7 +13325,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -13337,10 +13334,10 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13349,7 +13346,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13374,7 +13371,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13383,7 +13380,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13408,7 +13405,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13417,7 +13414,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13442,24 +13439,24 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
       <fill>
@@ -13468,7 +13465,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
       <fill>
@@ -13477,27 +13474,27 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
       <fill>
@@ -13506,7 +13503,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
       <fill>
@@ -13515,27 +13512,27 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </dxf>
     <dxf>
       <fill>
@@ -13544,20 +13541,20 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13566,7 +13563,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13583,7 +13580,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13592,7 +13589,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13601,7 +13598,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13618,7 +13615,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13627,7 +13624,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13636,7 +13633,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13653,7 +13650,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13662,7 +13659,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13671,7 +13668,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13696,7 +13693,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13713,7 +13710,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -13730,24 +13727,24 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </dxf>
     <dxf>
       <fill>
@@ -13756,7 +13753,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </dxf>
     <dxf>
       <fill>
@@ -13765,7 +13762,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </dxf>
     <dxf>
       <fill>
@@ -13789,7 +13786,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -14008,208 +14005,208 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Query_Job_Profession" displayName="Query_Job_Profession" ref="A1:B95" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="65" displayName="Query_Job_Profession" headerRowDxfId="66" id="1" insertRowShift="1" name="Query_Job_Profession" ref="A1:B95" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B95"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="JOB PROFESSION NAME" queryTableFieldId="1" dataDxfId="64"/>
-    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="63"/>
+    <tableColumn dataDxfId="64" id="1" name="JOB PROFESSION NAME" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="63" id="2" name="JOB POSITION CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Query_Affiliate_with_Multifinance" displayName="Query_Affiliate_with_Multifinance" ref="AB1:AC16" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="33" displayName="Query_Affiliate_with_Multifinance" headerRowDxfId="34" id="10" insertRowShift="1" name="Query_Affiliate_with_Multifinance" ref="AB1:AC16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AB1:AC16"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="AFFILIATE WITH MULTIFINANCE SLIK" queryTableFieldId="1" dataDxfId="32"/>
-    <tableColumn id="2" uniqueName="2" name="CODE" queryTableFieldId="2" dataDxfId="31"/>
+    <tableColumn dataDxfId="32" id="1" name="AFFILIATE WITH MULTIFINANCE SLIK" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="31" id="2" name="CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Query_Department_AML" displayName="Query_Department_AML" ref="AE1:AF492" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="29" displayName="Query_Department_AML" headerRowDxfId="30" id="11" insertRowShift="1" name="Query_Department_AML" ref="AE1:AF492" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AE1:AF492"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="DEPARTMENT AML" queryTableFieldId="1" dataDxfId="28"/>
-    <tableColumn id="2" uniqueName="2" name="DEPARTMENT AML CODE" queryTableFieldId="2" dataDxfId="27"/>
+    <tableColumn dataDxfId="28" id="1" name="DEPARTMENT AML" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="27" id="2" name="DEPARTMENT AML CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Query_csp_usl_source_aml" displayName="Query_csp_usl_source_aml" ref="AH1:AI10" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="25" displayName="Query_csp_usl_source_aml" headerRowDxfId="26" id="12" insertRowShift="1" name="Query_csp_usl_source_aml" ref="AH1:AI10" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AH1:AI10"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="CSP/USL SOURCE AML" queryTableFieldId="1" dataDxfId="24"/>
-    <tableColumn id="2" uniqueName="2" name="CSP/USL SOURCE AML CODE" queryTableFieldId="2" dataDxfId="23"/>
+    <tableColumn dataDxfId="24" id="1" name="CSP/USL SOURCE AML" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="23" id="2" name="CSP/USL SOURCE AML CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Query_payment_type_aml" displayName="Query_payment_type_aml" ref="AK1:AL3" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="21" displayName="Query_payment_type_aml" headerRowDxfId="22" id="13" insertRowShift="1" name="Query_payment_type_aml" ref="AK1:AL3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AK1:AL3"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="PAYMENT TYPE AML" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" uniqueName="2" name="CODE" queryTableFieldId="2" dataDxfId="19"/>
+    <tableColumn dataDxfId="20" id="1" name="PAYMENT TYPE AML" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="19" id="2" name="CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Query_authority_aml" displayName="Query_authority_aml" ref="AN1:AO9" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="17" displayName="Query_authority_aml" headerRowDxfId="18" id="14" insertRowShift="1" name="Query_authority_aml" ref="AN1:AO9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AN1:AO9"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="AUTHORITY AML" queryTableFieldId="1" dataDxfId="16"/>
-    <tableColumn id="2" uniqueName="2" name="AUTHORITY AML2" queryTableFieldId="2" dataDxfId="15"/>
+    <tableColumn dataDxfId="16" id="1" name="AUTHORITY AML" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="15" id="2" name="AUTHORITY AML2" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Query_Business_Source" displayName="Query_Business_Source" ref="AQ1:AR2" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="13" displayName="Query_Business_Source" headerRowDxfId="14" id="15" insertRowShift="1" name="Query_Business_Source" ref="AQ1:AR2" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AQ1:AR2"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="BUSINESS SOURCE AML" queryTableFieldId="1" dataDxfId="12"/>
-    <tableColumn id="2" uniqueName="2" name="CODE" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn dataDxfId="12" id="1" name="BUSINESS SOURCE AML" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="11" id="2" name="CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="query_building" displayName="query_building" ref="AT1:AU8" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="9" displayName="query_building" headerRowDxfId="10" id="16" insertRowShift="1" name="query_building" ref="AT1:AU8" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AT1:AU8"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="BUILDING" queryTableFieldId="1" dataDxfId="8"/>
-    <tableColumn id="2" uniqueName="2" name="BUILDING CODE" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn dataDxfId="8" id="1" name="BUILDING" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="7" id="2" name="BUILDING CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Query_Industry_Type" displayName="Query_Industry_Type" ref="AW1:AX263" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="5" displayName="Query_Industry_Type" headerRowDxfId="6" id="17" insertRowShift="1" name="Query_Industry_Type" ref="AW1:AX263" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AW1:AX263"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="INDUSTRY TYPE NAME" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" uniqueName="2" name="INDUSTRY TYPE CODE" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn dataDxfId="4" id="1" name="INDUSTRY TYPE NAME" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="3" id="2" name="INDUSTRY TYPE CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Query_Country" displayName="Query_Country" ref="BA1:BB242" tableType="queryTable" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Query_Country" headerRowDxfId="2" id="18" name="Query_Country" ref="BA1:BB242" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BA1:BB242"/>
   <tableColumns count="2">
-    <tableColumn id="5" uniqueName="5" name="COUNTRY NAME" queryTableFieldId="1"/>
-    <tableColumn id="6" uniqueName="6" name="COUNTRY CODE" queryTableFieldId="2"/>
+    <tableColumn id="5" name="COUNTRY NAME" queryTableFieldId="1" uniqueName="5"/>
+    <tableColumn id="6" name="COUNTRY CODE" queryTableFieldId="2" uniqueName="6"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Query_Copy_Address_From" displayName="Query_Copy_Address_From" ref="BE1:BE10" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Query_Copy_Address_From" headerRowDxfId="1" id="19" name="Query_Copy_Address_From" ref="BE1:BE10" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BE1:BE10"/>
   <tableColumns count="1">
-    <tableColumn id="3" uniqueName="3" name="Copy Address" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn dataDxfId="0" id="3" name="Copy Address" queryTableFieldId="1" uniqueName="3"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Query_Job_Position" displayName="Query_Job_Position" ref="E1:E30" tableType="queryTable" totalsRowShown="0" headerRowDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Query_Job_Position" headerRowDxfId="62" id="2" name="Query_Job_Position" ref="E1:E30" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="E1:E30"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="JOB POSITION NAME" queryTableFieldId="1" dataDxfId="61"/>
+    <tableColumn dataDxfId="61" id="1" name="JOB POSITION NAME" queryTableFieldId="1" uniqueName="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Query_Customer_Relationship" displayName="Query_Customer_Relationship" ref="H1:H14" tableType="queryTable" totalsRowShown="0" headerRowDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Query_Customer_Relationship" headerRowDxfId="60" id="3" name="Query_Customer_Relationship" ref="H1:H14" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="H1:H14"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Customer Relationship" queryTableFieldId="1" dataDxfId="59"/>
+    <tableColumn dataDxfId="59" id="1" name="Customer Relationship" queryTableFieldId="1" uniqueName="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Query_Bank" displayName="Query_Bank" ref="J1:K147" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="57" displayName="Query_Bank" headerRowDxfId="58" id="4" insertRowShift="1" name="Query_Bank" ref="J1:K147" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="J1:K147"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="BANK NAME" queryTableFieldId="1" dataDxfId="56"/>
-    <tableColumn id="2" uniqueName="2" name="BANK CODE" queryTableFieldId="2" dataDxfId="55"/>
+    <tableColumn dataDxfId="56" id="1" name="BANK NAME" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="55" id="2" name="BANK CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Query_Debtor_Group" displayName="Query_Debtor_Group" ref="M1:N315" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="53" displayName="Query_Debtor_Group" headerRowDxfId="54" id="5" insertRowShift="1" name="Query_Debtor_Group" ref="M1:N315" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="M1:N315"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="DEBTOR GROUP NAME" queryTableFieldId="1" dataDxfId="52"/>
-    <tableColumn id="2" uniqueName="2" name="DEBTOR GROUP CODE" queryTableFieldId="2" dataDxfId="51"/>
+    <tableColumn dataDxfId="52" id="1" name="DEBTOR GROUP NAME" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="51" id="2" name="DEBTOR GROUP CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Query_Debtor_Business_Scale" displayName="Query_Debtor_Business_Scale" ref="P1:Q6" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="49" displayName="Query_Debtor_Business_Scale" headerRowDxfId="50" id="6" insertRowShift="1" name="Query_Debtor_Business_Scale" ref="P1:Q6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="P1:Q6"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="Debtor Business Scale Description" queryTableFieldId="1" dataDxfId="48"/>
-    <tableColumn id="2" uniqueName="2" name="Debtor Group Code" queryTableFieldId="2" dataDxfId="47"/>
+    <tableColumn dataDxfId="48" id="1" name="Debtor Business Scale Description" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="47" id="2" name="Debtor Group Code" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Query_Counterpart" displayName="Query_Counterpart" ref="S1:T175" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="45" displayName="Query_Counterpart" headerRowDxfId="46" id="7" insertRowShift="1" name="Query_Counterpart" ref="S1:T175" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="S1:T175"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="Counterpart Category" queryTableFieldId="1" dataDxfId="44"/>
-    <tableColumn id="2" uniqueName="2" name="LBPP CODE" queryTableFieldId="2" dataDxfId="43"/>
+    <tableColumn dataDxfId="44" id="1" name="Counterpart Category" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="43" id="2" name="LBPP CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Query_Sustainable_Financial" displayName="Query_Sustainable_Financial" ref="V1:W14" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="41" displayName="Query_Sustainable_Financial" headerRowDxfId="42" id="8" insertRowShift="1" name="Query_Sustainable_Financial" ref="V1:W14" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="V1:W14"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="Sustainable Financial Business" queryTableFieldId="1" dataDxfId="40"/>
-    <tableColumn id="2" uniqueName="2" name="LBPP Code" queryTableFieldId="2" dataDxfId="39"/>
+    <tableColumn dataDxfId="40" id="1" name="Sustainable Financial Business" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="39" id="2" name="LBPP Code" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Query_debtor_group_slik" displayName="Query_debtor_group_slik" ref="Y1:Z193" tableType="queryTable" insertRowShift="1" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="37" displayName="Query_debtor_group_slik" headerRowDxfId="38" id="9" insertRowShift="1" name="Query_debtor_group_slik" ref="Y1:Z193" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="Y1:Z193"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="DEBTOR GROUP SLIK" queryTableFieldId="1" dataDxfId="36"/>
-    <tableColumn id="2" uniqueName="2" name="DEBTOR GROUP SLIK CODE" queryTableFieldId="2" dataDxfId="35"/>
+    <tableColumn dataDxfId="36" id="1" name="DEBTOR GROUP SLIK" queryTableFieldId="1" uniqueName="1"/>
+    <tableColumn dataDxfId="35" id="2" name="DEBTOR GROUP SLIK CODE" queryTableFieldId="2" uniqueName="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
@@ -14218,10 +14215,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -14256,7 +14253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -14291,7 +14288,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -14385,21 +14382,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -14416,7 +14413,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -14468,34 +14465,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>4175</v>
+        <v>4173</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3353</v>
@@ -14507,12 +14504,12 @@
         <v>3353</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4174</v>
+        <v>4177</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -14524,7 +14521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -14532,10 +14529,10 @@
         <v>4177</v>
       </c>
       <c r="C3" t="s">
-        <v>4176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4174</v>
+      </c>
+    </row>
+    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -14550,7 +14547,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -14565,7 +14562,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -14580,7 +14577,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -14597,7 +14594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -14614,7 +14611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -14631,15 +14628,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4166</v>
+      </c>
+    </row>
+    <row customFormat="1" r="11" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>14</v>
       </c>
@@ -14656,17 +14653,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="14" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>18</v>
       </c>
@@ -14683,7 +14680,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>3645</v>
       </c>
@@ -14704,7 +14701,7 @@
         <v>COUNTRY001</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>20</v>
       </c>
@@ -14727,47 +14724,45 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>4143</v>
+        <v>4142</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4143</v>
+        <v>4142</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>4143</v>
+        <v>4142</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>4143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4142</v>
+      </c>
+    </row>
+    <row customFormat="1" r="18" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4145</v>
+        <v>4144</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>4145</v>
+        <v>4144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>4145</v>
+        <v>4144</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>4145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4144</v>
+      </c>
+    </row>
+    <row customFormat="1" r="19" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>4139</v>
-      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
         <v>4131</v>
       </c>
@@ -14786,65 +14781,65 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15:XFD16">
-    <cfRule type="expression" dxfId="69" priority="2">
+    <cfRule dxfId="69" priority="2" type="expression">
       <formula>AND(A$14&lt;&gt;"Foreigner",A$14&lt;&gt;"",A$14&lt;&gt;"Nationality")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:XFD19">
-    <cfRule type="expression" dxfId="68" priority="1">
+    <cfRule dxfId="68" priority="1" type="expression">
       <formula>A$8="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:K18">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F18:K18" type="list">
       <formula1>"Buddha, Catholic, Christian, Hindu, Islam, Kong Hu Cu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:K17">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F17:K17" type="list">
       <formula1>"S1, S2, S3, SD, SMP, SMA"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B10:K10"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B7:K9">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="B10:K10"/>
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="B7:K9" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F14:K14">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="F14:K14" type="list">
       <formula1>"Local, Foreigner"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F11:K11">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="F11:K11" type="list">
       <formula1>"Mr, Mrs, Ms"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:E14">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B14:E14" type="list">
       <formula1>"Local, Foreigner"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:E11">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B11:E11" type="list">
       <formula1>"Mr, Mrs, Ms"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:E15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B15:E15" type="custom">
       <formula1>B$14="Foreigner"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19:E19">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B19:E19" type="custom">
       <formula1>B$8="Yes"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B5">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4:B5" type="whole">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+24</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16" type="list">
       <formula1>IF(B$14="Foreigner",ListCountry)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:E17">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B17:E17" type="list">
       <formula1>"S1, S2, S3, SD, SMP, SMA, D3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:E18">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B18:E18" type="list">
       <formula1>"Buddha, Catholic, Christian, Hindu, Islam, Kong Hu Cu, AGNOSTIK"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>IF(C$14="Foreigner",Master!$BA$2:$BA$342)</xm:f>
           </x14:formula1>
@@ -14857,8 +14852,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -14866,16 +14861,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="5" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>4142</v>
+        <v>4141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3353</v>
@@ -14887,7 +14882,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>25</v>
       </c>
@@ -14904,7 +14899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -14923,12 +14918,12 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4160</v>
+        <v>4159</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>29</v>
@@ -14946,7 +14941,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>32</v>
       </c>
@@ -14969,7 +14964,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>33</v>
       </c>
@@ -14992,7 +14987,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>34</v>
       </c>
@@ -15015,12 +15010,12 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4162</v>
+        <v>4161</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>36</v>
@@ -15038,12 +15033,12 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4161</v>
+        <v>4160</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>36</v>
@@ -15061,12 +15056,12 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4163</v>
+        <v>4162</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>290</v>
@@ -15084,7 +15079,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>291</v>
       </c>
@@ -15099,7 +15094,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>292</v>
       </c>
@@ -15114,7 +15109,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>293</v>
       </c>
@@ -15129,7 +15124,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="14" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>294</v>
       </c>
@@ -15144,7 +15139,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>295</v>
       </c>
@@ -15159,7 +15154,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>296</v>
       </c>
@@ -15174,7 +15169,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>297</v>
       </c>
@@ -15189,7 +15184,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>298</v>
       </c>
@@ -15204,7 +15199,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="19" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>299</v>
       </c>
@@ -15219,7 +15214,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="20" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>300</v>
       </c>
@@ -15234,7 +15229,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="21" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>301</v>
       </c>
@@ -15249,7 +15244,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="22" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>40</v>
       </c>
@@ -15268,36 +15263,36 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:XFD10">
-    <cfRule type="expression" dxfId="67" priority="1">
+    <cfRule dxfId="67" priority="1" type="expression">
       <formula>AND(A$3&lt;&gt;"",A$3&lt;&gt;"Copy Address From")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B22:K22">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="B22:K22" type="list">
       <formula1>"Dinas, Family, KPR, Rented, Self - Owned"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:K2">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="B2:K2" type="list">
       <formula1>"Legal, Mailing, Residence, Residence 2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:K3">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="I3:K3" type="list">
       <formula1>"Job, Legal, Residence"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B10">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4:B10" type="custom">
       <formula1>ISBLANK(B$3)</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$BE$2:$BE$110</xm:f>
           </x14:formula1>
           <xm:sqref>C3:H3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$BE$2:$BE$20</xm:f>
           </x14:formula1>
@@ -15310,25 +15305,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K114"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="2" max="5" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>4142</v>
+        <v>4141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3353</v>
@@ -15340,22 +15335,22 @@
         <v>3353</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+    <row customFormat="1" r="2" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
         <v>3633</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="48"/>
+    </row>
+    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>42</v>
       </c>
@@ -15382,7 +15377,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>99</v>
       </c>
@@ -15405,7 +15400,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>44</v>
       </c>
@@ -15428,15 +15423,15 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4140</v>
+        <v>4139</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4140</v>
+        <v>4139</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>48</v>
@@ -15451,7 +15446,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
@@ -15468,7 +15463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -15485,7 +15480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>280</v>
       </c>
@@ -15493,7 +15488,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>281</v>
       </c>
@@ -15511,7 +15506,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>282</v>
       </c>
@@ -15528,7 +15523,7 @@
         <v>3092</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -15542,7 +15537,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>54</v>
       </c>
@@ -15565,7 +15560,7 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="14" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>283</v>
       </c>
@@ -15586,7 +15581,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -15607,12 +15602,12 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
-        <v>4146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="45" t="s">
+        <v>4145</v>
+      </c>
+    </row>
+    <row customFormat="1" r="17" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>42</v>
       </c>
@@ -15633,7 +15628,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>99</v>
       </c>
@@ -15644,7 +15639,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="19" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -15652,14 +15647,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="20" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="21" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
-        <v>4147</v>
+        <v>4146</v>
       </c>
       <c r="B21" s="1" t="str">
         <f>VLOOKUP(B22,Master!$AW:$AX,2,FALSE)</f>
@@ -15678,31 +15673,31 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="22" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>4147</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>4148</v>
       </c>
-      <c r="B22" s="1" t="s">
+    </row>
+    <row customFormat="1" r="23" s="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>4149</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>4150</v>
       </c>
       <c r="B23" s="1">
         <v>1823612693</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="24" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>4151</v>
+        <v>4150</v>
       </c>
       <c r="B24" s="37">
         <v>44056</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>283</v>
       </c>
@@ -15710,12 +15705,12 @@
         <v>311</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
-        <v>4152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="26" s="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
+        <v>4151</v>
+      </c>
+    </row>
+    <row customFormat="1" r="27" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
         <v>42</v>
       </c>
@@ -15724,7 +15719,7 @@
         <v>CLG_STD</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="28" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>99</v>
       </c>
@@ -15732,17 +15727,17 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="29" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
-        <v>4153</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="30" s="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="45" t="s">
+        <v>4152</v>
+      </c>
+    </row>
+    <row customFormat="1" r="31" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>42</v>
       </c>
@@ -15751,7 +15746,7 @@
         <v>ENTR</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="32" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>99</v>
       </c>
@@ -15759,7 +15754,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="33" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>44</v>
       </c>
@@ -15767,7 +15762,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="34" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>50</v>
       </c>
@@ -15775,45 +15770,45 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="35" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>280</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>4154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4153</v>
+      </c>
+    </row>
+    <row customFormat="1" r="36" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>4147</v>
+        <v>4146</v>
       </c>
       <c r="B36" s="1" t="str">
         <f>VLOOKUP(B37,Master!$AW:$AX,2,FALSE)</f>
         <v>1119</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="37" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>4148</v>
+        <v>4147</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>4154</v>
+      </c>
+    </row>
+    <row customFormat="1" r="38" s="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>4155</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row customFormat="1" r="39" s="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>4156</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="36" t="s">
         <v>4157</v>
       </c>
-      <c r="B39" s="36" t="s">
-        <v>4158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row customFormat="1" r="40" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>283</v>
       </c>
@@ -15821,7 +15816,7 @@
         <v>3373</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="41" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -15829,32 +15824,32 @@
         <v>500</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="42" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>4159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="43" t="s">
+        <v>4158</v>
+      </c>
+    </row>
+    <row customFormat="1" r="43" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="46" t="s">
         <v>3634</v>
       </c>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="45"/>
-    </row>
-    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="48"/>
+    </row>
+    <row customFormat="1" r="44" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>28</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>4164</v>
+        <v>4163</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>29</v>
@@ -15866,7 +15861,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="45" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>32</v>
       </c>
@@ -15889,7 +15884,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="46" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
         <v>33</v>
       </c>
@@ -15912,7 +15907,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="47" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
         <v>34</v>
       </c>
@@ -15935,12 +15930,12 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="48" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
         <v>35</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>4144</v>
+        <v>4143</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>36</v>
@@ -15958,7 +15953,7 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="49" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
         <v>37</v>
       </c>
@@ -15981,7 +15976,7 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="50" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>38</v>
       </c>
@@ -16004,7 +15999,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="51" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>39</v>
       </c>
@@ -16019,7 +16014,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="52" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>291</v>
       </c>
@@ -16034,7 +16029,7 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="53" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>292</v>
       </c>
@@ -16049,7 +16044,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="54" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>293</v>
       </c>
@@ -16064,7 +16059,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="55" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>294</v>
       </c>
@@ -16079,7 +16074,7 @@
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="56" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>295</v>
       </c>
@@ -16094,7 +16089,7 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="57" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>296</v>
       </c>
@@ -16109,7 +16104,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="58" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>297</v>
       </c>
@@ -16124,7 +16119,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="59" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>298</v>
       </c>
@@ -16139,7 +16134,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="60" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>299</v>
       </c>
@@ -16154,7 +16149,7 @@
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="61" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>300</v>
       </c>
@@ -16169,7 +16164,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="62" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>301</v>
       </c>
@@ -16184,7 +16179,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="63" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>40</v>
       </c>
@@ -16198,53 +16193,53 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="43" t="s">
+    <row customFormat="1" r="64" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="46" t="s">
         <v>3635</v>
       </c>
-      <c r="B64" s="44"/>
-      <c r="C64" s="44"/>
-      <c r="D64" s="44"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="44"/>
-      <c r="G64" s="44"/>
-      <c r="H64" s="44"/>
-      <c r="I64" s="44"/>
-      <c r="J64" s="44"/>
-      <c r="K64" s="45"/>
-    </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="47"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="47"/>
+      <c r="H64" s="47"/>
+      <c r="I64" s="47"/>
+      <c r="J64" s="47"/>
+      <c r="K64" s="48"/>
+    </row>
+    <row customFormat="1" r="65" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="66" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>285</v>
       </c>
       <c r="B66" s="37"/>
     </row>
-    <row r="67" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="43" t="s">
+    <row customFormat="1" r="67" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="46" t="s">
         <v>3636</v>
       </c>
-      <c r="B67" s="44"/>
-      <c r="C67" s="44"/>
-      <c r="D67" s="44"/>
-      <c r="E67" s="44"/>
-      <c r="F67" s="44"/>
-      <c r="G67" s="44"/>
-      <c r="H67" s="44"/>
-      <c r="I67" s="44"/>
-      <c r="J67" s="44"/>
-      <c r="K67" s="45"/>
-    </row>
-    <row r="68" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="47"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="47"/>
+      <c r="J67" s="47"/>
+      <c r="K67" s="48"/>
+    </row>
+    <row customFormat="1" r="68" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>345</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>4172</v>
+        <v>4171</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>29</v>
@@ -16256,7 +16251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="69" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>346</v>
       </c>
@@ -16279,7 +16274,7 @@
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="70" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>347</v>
       </c>
@@ -16302,7 +16297,7 @@
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="71" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>348</v>
       </c>
@@ -16325,12 +16320,12 @@
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="72" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>349</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>4169</v>
+        <v>4168</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>36</v>
@@ -16348,12 +16343,12 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="73" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>350</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>4170</v>
+        <v>4169</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>36</v>
@@ -16371,12 +16366,12 @@
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="74" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>351</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>4171</v>
+        <v>4170</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>290</v>
@@ -16394,7 +16389,7 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="75" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>352</v>
       </c>
@@ -16409,7 +16404,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="76" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>353</v>
       </c>
@@ -16424,7 +16419,7 @@
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="77" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>354</v>
       </c>
@@ -16439,7 +16434,7 @@
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="78" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>355</v>
       </c>
@@ -16454,7 +16449,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="79" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>356</v>
       </c>
@@ -16469,7 +16464,7 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="80" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>357</v>
       </c>
@@ -16484,7 +16479,7 @@
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="81" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>358</v>
       </c>
@@ -16499,7 +16494,7 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="82" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>359</v>
       </c>
@@ -16514,7 +16509,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="83" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>360</v>
       </c>
@@ -16529,7 +16524,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="84" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>361</v>
       </c>
@@ -16544,7 +16539,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="85" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>362</v>
       </c>
@@ -16559,7 +16554,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="86" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>363</v>
       </c>
@@ -16574,7 +16569,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="87" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>364</v>
       </c>
@@ -16588,63 +16583,63 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="43" t="s">
+    <row customFormat="1" r="88" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="46" t="s">
         <v>3637</v>
       </c>
-      <c r="B88" s="44"/>
-      <c r="C88" s="44"/>
-      <c r="D88" s="44"/>
-      <c r="E88" s="44"/>
-      <c r="F88" s="44"/>
-      <c r="G88" s="44"/>
-      <c r="H88" s="44"/>
-      <c r="I88" s="44"/>
-      <c r="J88" s="44"/>
-      <c r="K88" s="45"/>
-    </row>
-    <row r="89" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="47"/>
+      <c r="C88" s="47"/>
+      <c r="D88" s="47"/>
+      <c r="E88" s="47"/>
+      <c r="F88" s="47"/>
+      <c r="G88" s="47"/>
+      <c r="H88" s="47"/>
+      <c r="I88" s="47"/>
+      <c r="J88" s="47"/>
+      <c r="K88" s="48"/>
+    </row>
+    <row customFormat="1" r="89" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="90" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="91" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="91" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="92" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="93" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>289</v>
       </c>
       <c r="B93" s="37"/>
     </row>
-    <row r="94" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="43" t="s">
+    <row customFormat="1" r="94" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="46" t="s">
         <v>3638</v>
       </c>
-      <c r="B94" s="44"/>
-      <c r="C94" s="44"/>
-      <c r="D94" s="44"/>
-      <c r="E94" s="44"/>
-      <c r="F94" s="44"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="44"/>
-      <c r="I94" s="44"/>
-      <c r="J94" s="44"/>
-      <c r="K94" s="45"/>
-    </row>
-    <row r="95" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="47"/>
+      <c r="C94" s="47"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47"/>
+      <c r="F94" s="47"/>
+      <c r="G94" s="47"/>
+      <c r="H94" s="47"/>
+      <c r="I94" s="47"/>
+      <c r="J94" s="47"/>
+      <c r="K94" s="48"/>
+    </row>
+    <row customFormat="1" r="95" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>325</v>
       </c>
@@ -16658,7 +16653,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="96" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>326</v>
       </c>
@@ -16679,7 +16674,7 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="97" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>327</v>
       </c>
@@ -16700,7 +16695,7 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="98" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>328</v>
       </c>
@@ -16721,7 +16716,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="99" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>329</v>
       </c>
@@ -16735,7 +16730,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="100" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="100" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>330</v>
       </c>
@@ -16749,7 +16744,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="101" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>331</v>
       </c>
@@ -16763,7 +16758,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="102" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>332</v>
       </c>
@@ -16778,7 +16773,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="103" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>333</v>
       </c>
@@ -16793,7 +16788,7 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="104" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>334</v>
       </c>
@@ -16808,7 +16803,7 @@
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
     </row>
-    <row r="105" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="105" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>335</v>
       </c>
@@ -16823,7 +16818,7 @@
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="106" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>336</v>
       </c>
@@ -16838,7 +16833,7 @@
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="107" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>337</v>
       </c>
@@ -16853,7 +16848,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
     </row>
-    <row r="108" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="108" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>338</v>
       </c>
@@ -16868,7 +16863,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="109" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>339</v>
       </c>
@@ -16883,7 +16878,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
     </row>
-    <row r="110" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="110" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>340</v>
       </c>
@@ -16898,7 +16893,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
     </row>
-    <row r="111" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="111" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>341</v>
       </c>
@@ -16913,7 +16908,7 @@
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
     </row>
-    <row r="112" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="112" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>342</v>
       </c>
@@ -16928,7 +16923,7 @@
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
     </row>
-    <row r="113" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="113" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>343</v>
       </c>
@@ -16943,7 +16938,7 @@
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
     </row>
-    <row r="114" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="114" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>344</v>
       </c>
@@ -16970,60 +16965,60 @@
     <mergeCell ref="A88:XFD88"/>
   </mergeCells>
   <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:K8 F11:K11 B19:E19 B34">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:K8 F11:K11 B19:E19 B34" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C87:K87 C63:K63 C114:K114">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="C87:K87 C63:K63 C114:K114" type="list">
       <formula1>"Dinas, Family, KPR, Rented, Self - Owned"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:K6">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6:K6" type="list">
       <formula1>"Contract, Permanent"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B41">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B15 B41" type="whole">
       <formula1>0</formula1>
       <formula2>999999999999999000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 B18:E18 B32 B28">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4 B18:E18 B32 B28" type="list">
       <formula1>ListJobProfession</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 B33">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B5 B33" type="list">
       <formula1>ListJobPosition</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B22:E22 B37">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B11 B22:E22 B37" type="list">
       <formula1>ListIndustryType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63 B87 B114">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B63 B87 B114" type="list">
       <formula1>"Dinas, Family, KPR, Rented, Self - Owned"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B42" type="list">
       <formula1>"Domestic Investment, Foreign Investment"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>F5:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$A$2:$A$195</xm:f>
           </x14:formula1>
           <xm:sqref>C4:E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$E$2:$E$129</xm:f>
           </x14:formula1>
           <xm:sqref>C5:E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$AW$2:$AW$515</xm:f>
           </x14:formula1>
@@ -17036,8 +17031,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -17045,19 +17040,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>4142</v>
+        <v>4141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3353</v>
@@ -17069,7 +17064,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>365</v>
       </c>
@@ -17077,7 +17072,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>58</v>
       </c>
@@ -17100,7 +17095,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>62</v>
       </c>
@@ -17123,7 +17118,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -17136,22 +17131,22 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F3:K3">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="F3:K3" type="list">
       <formula1>"AKTA, CAT CAT, CAT IS A CAT, DESCRIPTION FOR AAA, DESCRIPTION FOR ASA, DESCRIPTION FOR KTP, E-KTP, KITAS, NPWP, SIM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:E5">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B5:E5" type="list">
       <formula1>"Job, Legal, Residence"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4" type="list">
       <formula1>ListCusRel</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$H$2:$H$113</xm:f>
           </x14:formula1>
@@ -17164,25 +17159,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="2" max="5" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>4175</v>
+        <v>4141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3353</v>
@@ -17194,22 +17189,22 @@
         <v>3353</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+    <row customFormat="1" r="2" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
         <v>3639</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="48"/>
+    </row>
+    <row customFormat="1" r="3" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>65</v>
       </c>
@@ -17232,7 +17227,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
@@ -17253,7 +17248,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>67</v>
       </c>
@@ -17276,7 +17271,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
@@ -17297,7 +17292,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
@@ -17318,7 +17313,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>379</v>
       </c>
@@ -17341,14 +17336,16 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>4178</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+        <v>4175</v>
+      </c>
+      <c r="B9" s="38">
+        <v>3000000</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -17356,37 +17353,39 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>4179</v>
-      </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+    <row customFormat="1" r="10" s="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>4176</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+    </row>
+    <row customFormat="1" r="11" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
         <v>3640</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="48"/>
+    </row>
+    <row customFormat="1" r="12" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>73</v>
       </c>
@@ -17409,27 +17408,28 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+    <row customFormat="1" r="13" s="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
         <v>3641</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="45"/>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="48"/>
+    </row>
+    <row customFormat="1" r="14" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="3">
-        <v>192974891</v>
+      <c r="B14" s="3" t="str">
+        <f>VLOOKUP(B15,Master!$J$1:$K$204,2,FALSE)</f>
+        <v>014</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>VLOOKUP(C15,Master!$J$1:$K$204,2,FALSE)</f>
@@ -17450,7 +17450,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>728</v>
       </c>
@@ -17473,12 +17473,12 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4166</v>
+        <v>4165</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>77</v>
@@ -17490,12 +17490,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>4165</v>
+        <v>4164</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>79</v>
@@ -17507,12 +17507,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>4168</v>
+        <v>4167</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>82</v>
@@ -17530,7 +17530,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="19" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>83</v>
       </c>
@@ -17547,7 +17547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="20" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>84</v>
       </c>
@@ -17564,7 +17564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="21" s="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>729</v>
       </c>
@@ -17582,42 +17582,42 @@
     <mergeCell ref="A13:XFD13"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G19:K21 B19:F20">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G19:K21 B19:F20" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:K5">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B5:K5" type="list">
       <formula1>"Business, Online Shop, Salary, Stock Trading"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B3:B4" type="whole">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+27</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6:B7" type="whole">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+22</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12" type="whole">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+24</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B21" type="whole">
       <formula1>0</formula1>
       <formula2>9.99999999999999E+23</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B15" type="list">
       <formula1>ListBank</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10:E10">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="B10:E10" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$J$2:$J$305</xm:f>
           </x14:formula1>
@@ -17630,8 +17630,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -17639,16 +17639,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="5" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>4142</v>
+        <v>4141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3353</v>
@@ -17660,7 +17660,7 @@
         <v>3353</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>85</v>
       </c>
@@ -17674,7 +17674,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -17688,7 +17688,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>89</v>
       </c>
@@ -17703,7 +17703,7 @@
         <v>600000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>90</v>
       </c>
@@ -17720,21 +17720,21 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:E2">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:E2" type="list">
       <formula1>"Mobil, Motor, Rumah"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:E5">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4:E5" type="whole">
       <formula1>0</formula1>
       <formula2>999999999999999000000</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
@@ -17742,17 +17742,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" style="7" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="14.85546875" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="7" width="15.0" collapsed="true"/>
+    <col min="3" max="5" bestFit="true" customWidth="true" style="7" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>4175</v>
+        <v>4173</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3353</v>
@@ -17764,16 +17764,16 @@
         <v>3353</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+    <row customFormat="1" r="2" s="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
         <v>3642</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45"/>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
+    </row>
+    <row customFormat="1" r="3" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>91</v>
       </c>
@@ -17794,7 +17794,7 @@
         <v>07</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>730</v>
       </c>
@@ -17811,7 +17811,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>96</v>
       </c>
@@ -17832,7 +17832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>731</v>
       </c>
@@ -17849,7 +17849,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>1467</v>
       </c>
@@ -17870,7 +17870,7 @@
         <v>e2955</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="135" r="8" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>732</v>
       </c>
@@ -17887,7 +17887,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>1468</v>
       </c>
@@ -17908,7 +17908,7 @@
         <v>e3822</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="105" r="10" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>733</v>
       </c>
@@ -17925,27 +17925,27 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+    <row customFormat="1" r="11" s="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
         <v>3643</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
+    </row>
+    <row customFormat="1" r="12" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1649</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>4141</v>
+        <v>4140</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>1650</v>
       </c>
@@ -17966,7 +17966,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="14" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>1651</v>
       </c>
@@ -17977,29 +17977,29 @@
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1652</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>4141</v>
+        <v>4140</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1653</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>4141</v>
+        <v>4140</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>1657</v>
       </c>
@@ -18020,7 +18020,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="18" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>1654</v>
       </c>
@@ -18031,7 +18031,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="19" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>1656</v>
       </c>
@@ -18052,7 +18052,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="20" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>1655</v>
       </c>
@@ -18063,7 +18063,7 @@
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="21" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
         <v>1659</v>
       </c>
@@ -18084,7 +18084,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="22" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>1658</v>
       </c>
@@ -18095,7 +18095,7 @@
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="23" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>1660</v>
       </c>
@@ -18116,7 +18116,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="24" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>1661</v>
       </c>
@@ -18127,18 +18127,18 @@
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>1662</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>4141</v>
+        <v>4140</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="26" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>1663</v>
       </c>
@@ -18159,7 +18159,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="27" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1664</v>
       </c>
@@ -18168,7 +18168,7 @@
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="28" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>97</v>
       </c>
@@ -18185,7 +18185,7 @@
         <v>3355</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="29" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>1665</v>
       </c>
@@ -18206,7 +18206,7 @@
         <v>BISNIS_SENDIRI</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="30" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>1666</v>
       </c>
@@ -18223,7 +18223,7 @@
         <v>3055</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="31" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>1667</v>
       </c>
@@ -18240,12 +18240,12 @@
         <v>3354</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="32" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>1668</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>4173</v>
+        <v>4172</v>
       </c>
       <c r="C32" s="10" t="str">
         <f>VLOOKUP(C33,Master!$AT:$AU,2,FALSE)</f>
@@ -18260,7 +18260,7 @@
         <v>FAMILY</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="33" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>1669</v>
       </c>
@@ -18283,121 +18283,121 @@
     <mergeCell ref="A11:XFD11"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:E16 C12:E12 C25:E25">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C15:E16 C12:E12 C25:E25" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12 B15:B16 B25">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B12 B15:B16 B25" type="list">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B4" type="list">
       <formula1>ListDebtGroup</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6" type="list">
       <formula1>ListDebtorBusinessScale</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8" type="list">
       <formula1>ListCounterpart</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10" type="list">
       <formula1>ListSusFinBus</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B14" type="list">
       <formula1>ListDebtGroupSLIK</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B18" type="list">
       <formula1>ListAfWiMult</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B20" type="list">
       <formula1>ListDeptAML</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B22" type="list">
       <formula1>ListCSPUSL</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B24" type="list">
       <formula1>ListPaymentTypeAML</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B27" type="list">
       <formula1>ListAuthorityAML</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B30" type="list">
       <formula1>ListBusinessSource</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B33" type="list">
       <formula1>ListBuilding</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$AT$2:$AT$109</xm:f>
           </x14:formula1>
           <xm:sqref>C33:E33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$M$2:$M$629</xm:f>
           </x14:formula1>
           <xm:sqref>C4:E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$P$2:$P$107</xm:f>
           </x14:formula1>
           <xm:sqref>C6:E6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$S$2:$S$349</xm:f>
           </x14:formula1>
           <xm:sqref>C8:E8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$V$2:$V$115</xm:f>
           </x14:formula1>
           <xm:sqref>C10:E10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$Y$2:$Y$385</xm:f>
           </x14:formula1>
           <xm:sqref>C14:E14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$AB$2:$AB$117</xm:f>
           </x14:formula1>
           <xm:sqref>C18:E18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$AE$2:$AE$983</xm:f>
           </x14:formula1>
           <xm:sqref>C20:E20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$AH$2:$AH$111</xm:f>
           </x14:formula1>
           <xm:sqref>C22:E22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$AK$2:$AK$104</xm:f>
           </x14:formula1>
           <xm:sqref>C24:E24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$AN$2:$AN$111</xm:f>
           </x14:formula1>
           <xm:sqref>C27:E27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
           <x14:formula1>
             <xm:f>Master!$AQ$2:$AQ$102</xm:f>
           </x14:formula1>
@@ -18410,8 +18410,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DB882"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DC882"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D92" sqref="D92"/>
@@ -18419,46 +18419,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" style="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30" style="17" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.85546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.85546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.85546875" style="19" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="29.42578125" style="17" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.85546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="33.85546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.7109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="255.7109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.85546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="80.140625" style="22" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="80.7109375" style="23" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="21.5703125" style="20" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="79.85546875" style="23" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="8.140625" style="20" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="89" style="17" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="25.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="23" style="17" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5703125" style="20" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="25.140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="31.140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="12.42578125" style="17" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="17.42578125" style="17" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="9.140625" style="17" collapsed="1"/>
-    <col min="49" max="49" width="97.7109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="22.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="15" width="42.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="17" width="30.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="17" width="23.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="17" width="35.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="19" width="18.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="17" width="29.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="17" width="22.85546875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="17" width="33.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="17" width="20.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="17" width="255.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="17" width="12.85546875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="22" width="80.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="17" width="12.5703125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="23" width="80.7109375" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="20" width="21.5703125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="23" width="79.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="20" width="8.140625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="17" width="89.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="17" width="25.5703125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="17" width="23.0" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" style="20" width="28.5703125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="17" width="25.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" style="17" width="31.140625" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="44" max="44" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="17" width="12.42578125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="17" width="17.42578125" collapsed="true"/>
+    <col min="48" max="48" style="17" width="9.140625" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" style="17" width="97.7109375" collapsed="true"/>
+    <col min="50" max="50" customWidth="true" style="17" width="22.5703125" collapsed="true"/>
+    <col min="53" max="53" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="54" max="54" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="57" max="57" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>3361</v>
       </c>
@@ -19343,7 +19343,7 @@
         <v>4137</v>
       </c>
     </row>
-    <row r="10" spans="1:57" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>115</v>
       </c>
@@ -19422,7 +19422,7 @@
         <v>4138</v>
       </c>
     </row>
-    <row r="11" spans="1:57" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>117</v>
       </c>
@@ -19490,7 +19490,7 @@
         <v>3667</v>
       </c>
     </row>
-    <row r="12" spans="1:57" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>119</v>
       </c>
@@ -22854,7 +22854,7 @@
         <v>3797</v>
       </c>
     </row>
-    <row r="77" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="77" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
         <v>247</v>
       </c>
@@ -22904,7 +22904,7 @@
         <v>3799</v>
       </c>
     </row>
-    <row r="78" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="78" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
         <v>249</v>
       </c>
@@ -23504,7 +23504,7 @@
         <v>3823</v>
       </c>
     </row>
-    <row r="90" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="90" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
         <v>271</v>
       </c>
@@ -23554,7 +23554,7 @@
         <v>3825</v>
       </c>
     </row>
-    <row r="91" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="91" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
         <v>272</v>
       </c>
@@ -24131,7 +24131,7 @@
         <v>3372</v>
       </c>
     </row>
-    <row r="103" spans="10:106" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="103" spans="10:106" x14ac:dyDescent="0.25">
       <c r="J103" s="18" t="s">
         <v>489</v>
       </c>
@@ -24175,7 +24175,7 @@
         <v>3851</v>
       </c>
     </row>
-    <row r="104" spans="10:106" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="104" spans="10:106" x14ac:dyDescent="0.25">
       <c r="J104" s="18" t="s">
         <v>390</v>
       </c>
@@ -24395,7 +24395,7 @@
         <v>3861</v>
       </c>
     </row>
-    <row r="109" spans="10:106" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="109" spans="10:106" x14ac:dyDescent="0.25">
       <c r="J109" s="18" t="s">
         <v>410</v>
       </c>
@@ -24659,7 +24659,7 @@
         <v>3873</v>
       </c>
     </row>
-    <row r="115" spans="10:54" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="115" spans="10:54" x14ac:dyDescent="0.25">
       <c r="J115" s="18" t="s">
         <v>509</v>
       </c>
@@ -24703,7 +24703,7 @@
         <v>3875</v>
       </c>
     </row>
-    <row r="116" spans="10:54" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="116" spans="10:54" x14ac:dyDescent="0.25">
       <c r="J116" s="18" t="s">
         <v>511</v>
       </c>
@@ -25671,7 +25671,7 @@
         <v>3919</v>
       </c>
     </row>
-    <row r="138" spans="10:54" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="138" spans="10:54" x14ac:dyDescent="0.25">
       <c r="J138" s="18" t="s">
         <v>550</v>
       </c>
@@ -26267,7 +26267,7 @@
         <v>3947</v>
       </c>
     </row>
-    <row r="152" spans="10:54" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="152" spans="10:54" x14ac:dyDescent="0.25">
       <c r="K152" s="20"/>
       <c r="M152" s="18" t="s">
         <v>884</v>
@@ -26306,7 +26306,7 @@
         <v>3949</v>
       </c>
     </row>
-    <row r="153" spans="10:54" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="153" spans="10:54" x14ac:dyDescent="0.25">
       <c r="K153" s="20"/>
       <c r="M153" s="18" t="s">
         <v>885</v>
@@ -33162,8 +33162,8 @@
       <c r="AF882" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <tableParts count="19">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
AITATR3- 87 + 84
</commit_message>
<xml_diff>
--- a/Excel/3. CustomerDataCompletion-Personal - Customer.xlsx
+++ b/Excel/3. CustomerDataCompletion-Personal - Customer.xlsx
@@ -12919,9 +12919,6 @@
     <t>BLI GUNG</t>
   </si>
   <si>
-    <t>vino</t>
-  </si>
-  <si>
     <t>Christian</t>
   </si>
   <si>
@@ -12932,6 +12929,9 @@
   </si>
   <si>
     <t>21836123697</t>
+  </si>
+  <si>
+    <t>kennedy</t>
   </si>
 </sst>
 </file>
@@ -14476,7 +14476,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14526,7 +14526,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>4173</v>
+        <v>4177</v>
       </c>
       <c r="C3" t="s">
         <v>4169</v>
@@ -14726,7 +14726,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>4175</v>
+        <v>4174</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4142</v>
@@ -14743,7 +14743,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4174</v>
+        <v>4173</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4144</v>
@@ -17495,7 +17495,7 @@
         <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>4176</v>
+        <v>4175</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>79</v>
@@ -17512,7 +17512,7 @@
         <v>80</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>4177</v>
+        <v>4176</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>82</v>

</xml_diff>